<commit_message>
client aristocrat is connected
</commit_message>
<xml_diff>
--- a/template/Report.xlsx
+++ b/template/Report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr codeName="ЭтаКнига"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
+  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\analytics\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="547"/>
   </bookViews>
@@ -443,12 +448,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00&quot;р.&quot;"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00&quot;р.&quot;"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -806,8 +811,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -836,7 +841,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1064,72 +1069,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1145,19 +1084,103 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1172,28 +1195,10 @@
     <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1226,7 +1231,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1280,6 +1285,23 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1327,7 +1349,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1368,7 +1390,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1409,7 +1431,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1450,7 +1472,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1491,7 +1513,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1532,7 +1554,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1585,7 +1607,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -1607,7 +1629,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
             </c:ext>
@@ -1703,7 +1725,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1745,7 +1767,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1760,7 +1782,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1788,7 +1810,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1803,7 +1825,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1831,7 +1853,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1846,7 +1868,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1952,7 +1974,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1994,7 +2016,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2012,12 +2034,12 @@
             <c:numRef>
               <c:f>[0]!sendall2</c:f>
               <c:numCache>
-                <c:formatCode>_("р."* #,##0.00_);_("р."* \(#,##0.00\);_("р."* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #\ ##0.00"р."_-;\-* #\ ##0.00"р."_-;_-* "-"??"р."_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2045,7 +2067,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2063,12 +2085,12 @@
             <c:numRef>
               <c:f>[0]!costConversation</c:f>
               <c:numCache>
-                <c:formatCode>_("р."* #,##0.00_);_("р."* \(#,##0.00\);_("р."* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #\ ##0.00"р."_-;\-* #\ ##0.00"р."_-;_-* "-"??"р."_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2096,7 +2118,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2119,7 +2141,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2162,7 +2184,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="_(&quot;р.&quot;* #,##0.00_);_(&quot;р.&quot;* \(#,##0.00\);_(&quot;р.&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #\ ##0.00&quot;р.&quot;_-;\-* #\ ##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2173,7 +2195,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2206,7 +2227,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2267,7 +2288,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1FE8-4CC8-A3E6-CD574745982A}"/>
             </c:ext>
@@ -2428,7 +2449,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2467,7 +2488,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-5B18-40B8-9E6F-B2250215750F}"/>
               </c:ext>
@@ -2487,7 +2508,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-5B18-40B8-9E6F-B2250215750F}"/>
               </c:ext>
@@ -2508,14 +2529,14 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="+mj-lt"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -2544,7 +2565,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -2566,7 +2587,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-5B18-40B8-9E6F-B2250215750F}"/>
             </c:ext>
@@ -2593,7 +2614,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2614,7 +2634,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Ubuntu" panose="020B0504030602030204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="+mj-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -2656,7 +2676,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2710,7 +2730,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6DCE-4170-A8BA-4BE124766687}"/>
             </c:ext>
@@ -2769,7 +2789,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -2822,7 +2842,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6DCE-4170-A8BA-4BE124766687}"/>
             </c:ext>
@@ -2958,7 +2978,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3021,7 +3040,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3058,7 +3077,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3080,7 +3099,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9533-424E-9DFF-B9454BE51E98}"/>
             </c:ext>
@@ -3100,7 +3119,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3133,7 +3151,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3185,7 +3203,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3209,7 +3227,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1C8B-4851-BE55-E5C0FF949603}"/>
             </c:ext>
@@ -3247,7 +3265,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3271,7 +3289,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1C8B-4851-BE55-E5C0FF949603}"/>
             </c:ext>
@@ -3326,7 +3344,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3342,7 +3359,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3373,7 +3390,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3388,7 +3404,7 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:explosion val="6"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-1576-4393-8E4F-7B3A075ADDFE}"/>
               </c:ext>
@@ -3409,7 +3425,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3431,7 +3447,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1576-4393-8E4F-7B3A075ADDFE}"/>
             </c:ext>
@@ -3467,7 +3483,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3510,7 +3526,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3EA3-48D1-8E98-DC97D53A6E0F}"/>
             </c:ext>
@@ -3540,7 +3556,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3EA3-48D1-8E98-DC97D53A6E0F}"/>
             </c:ext>
@@ -3594,7 +3610,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3627,7 +3642,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3661,7 +3676,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5324-4B7B-AB47-40E0FE10B1A4}"/>
             </c:ext>
@@ -3682,7 +3697,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5324-4B7B-AB47-40E0FE10B1A4}"/>
             </c:ext>
@@ -3735,7 +3750,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -7119,13 +7133,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AFF118AE-0192-452D-9AB7-AD9749DBEBF5}" type="pres">
       <dgm:prSet presAssocID="{D0B5C048-8C24-4F76-8C9D-7762D594F997}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7135,13 +7142,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{79388EF3-A8BE-4117-ACBA-8A08FF47472A}" type="pres">
       <dgm:prSet presAssocID="{A43066EC-58A2-4A7D-AF6B-37D46EA26464}" presName="Name8" presStyleCnt="0"/>
@@ -7155,13 +7155,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{673D1501-484B-4334-879E-3653F69F415A}" type="pres">
       <dgm:prSet presAssocID="{A43066EC-58A2-4A7D-AF6B-37D46EA26464}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7171,13 +7164,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{47D67E14-1695-4B93-9EB1-4CC623CC53C2}" type="pres">
       <dgm:prSet presAssocID="{93154AA3-294E-4A72-A452-A70CA494AC1C}" presName="Name8" presStyleCnt="0"/>
@@ -7191,13 +7177,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{E32FEE9D-FC56-4633-B235-BB4BC8FB2096}" type="pres">
       <dgm:prSet presAssocID="{93154AA3-294E-4A72-A452-A70CA494AC1C}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7207,13 +7186,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8AAD1D77-9DFF-4406-995B-9E373EE560D6}" type="pres">
       <dgm:prSet presAssocID="{6F6CEB40-F018-40B7-B43C-BB0F608C1737}" presName="Name8" presStyleCnt="0"/>
@@ -7227,13 +7199,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{166B6DC3-E48C-470D-B319-D777F3D4DA8C}" type="pres">
       <dgm:prSet presAssocID="{6F6CEB40-F018-40B7-B43C-BB0F608C1737}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7243,13 +7208,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7A3E38AC-ABE0-44B1-ABFE-C71AA69B5E79}" type="pres">
       <dgm:prSet presAssocID="{DFB816DE-9FE1-4A03-BBE3-E92EDD0106A3}" presName="Name8" presStyleCnt="0"/>
@@ -7263,13 +7221,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{53E7FBCA-B0EF-4CD3-9E52-80F3A839A7EA}" type="pres">
       <dgm:prSet presAssocID="{DFB816DE-9FE1-4A03-BBE3-E92EDD0106A3}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7279,13 +7230,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{40A0CFF3-5D9A-46B0-B3E9-C705D72172EE}" type="pres">
       <dgm:prSet presAssocID="{9672259E-8D62-4911-A026-2E23FD52D48A}" presName="Name8" presStyleCnt="0"/>
@@ -7299,13 +7243,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{22C6AEA5-B4B3-41C7-AE03-AA0A4D4EB3BF}" type="pres">
       <dgm:prSet presAssocID="{9672259E-8D62-4911-A026-2E23FD52D48A}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7315,13 +7252,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
@@ -7388,12 +7318,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="0" y="200912"/>
-          <a:ext cx="5136057" cy="774050"/>
+          <a:off x="0" y="200482"/>
+          <a:ext cx="5225704" cy="772392"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 52847"/>
+            <a:gd name="adj" fmla="val 53885"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7439,7 +7369,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7449,6 +7379,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7462,8 +7393,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="898809" y="200912"/>
-        <a:ext cx="3338437" cy="774050"/>
+        <a:off x="914498" y="200482"/>
+        <a:ext cx="3396707" cy="772392"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{69CA1DAA-1002-439B-95E6-9B03B9A978F9}">
@@ -7473,12 +7404,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="165705" y="930315"/>
-          <a:ext cx="4804646" cy="774050"/>
+          <a:off x="168597" y="928323"/>
+          <a:ext cx="4888508" cy="772392"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 52847"/>
+            <a:gd name="adj" fmla="val 53885"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7526,7 +7457,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7536,6 +7467,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7549,8 +7481,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1006518" y="930315"/>
-        <a:ext cx="3123020" cy="774050"/>
+        <a:off x="1024086" y="928323"/>
+        <a:ext cx="3177530" cy="772392"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{238952AD-046B-41C1-B6E4-2C5149FAC37B}">
@@ -7560,12 +7492,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="369890" y="1670880"/>
-          <a:ext cx="4396276" cy="774050"/>
+          <a:off x="376346" y="1667302"/>
+          <a:ext cx="4473010" cy="772392"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 52847"/>
+            <a:gd name="adj" fmla="val 53885"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7613,7 +7545,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7623,6 +7555,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7636,8 +7569,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1139238" y="1670880"/>
-        <a:ext cx="2857579" cy="774050"/>
+        <a:off x="1159123" y="1667302"/>
+        <a:ext cx="2907457" cy="772392"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{425953AF-BAA2-4E7A-916B-2A82294152AD}">
@@ -7647,12 +7580,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="609118" y="2400284"/>
-          <a:ext cx="3917819" cy="774050"/>
+          <a:off x="619750" y="2395144"/>
+          <a:ext cx="3986202" cy="772392"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 52847"/>
+            <a:gd name="adj" fmla="val 53885"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7700,7 +7633,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7710,6 +7643,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7723,8 +7657,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1294737" y="2400284"/>
-        <a:ext cx="2546582" cy="774050"/>
+        <a:off x="1317336" y="2395144"/>
+        <a:ext cx="2591031" cy="772392"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{5A06E787-2B65-46E6-9A04-2968475748A6}">
@@ -7734,12 +7668,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="872899" y="3129687"/>
-          <a:ext cx="3390258" cy="774050"/>
+          <a:off x="888135" y="3122985"/>
+          <a:ext cx="3449433" cy="772392"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 52847"/>
+            <a:gd name="adj" fmla="val 53885"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7787,7 +7721,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7797,6 +7731,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7810,8 +7745,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1466194" y="3129687"/>
-        <a:ext cx="2203667" cy="774050"/>
+        <a:off x="1491786" y="3122985"/>
+        <a:ext cx="2242131" cy="772392"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9D67B753-3B31-4AF4-8047-2E5F38D41F74}">
@@ -7821,12 +7756,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1028418" y="3870252"/>
-          <a:ext cx="3079220" cy="989097"/>
+          <a:off x="1046368" y="3861964"/>
+          <a:ext cx="3132966" cy="986979"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 52847"/>
+            <a:gd name="adj" fmla="val 53885"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7871,7 +7806,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7881,6 +7816,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="2000" kern="1200">
@@ -7903,8 +7839,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1028418" y="3870252"/>
-        <a:ext cx="3079220" cy="989097"/>
+        <a:off x="1046368" y="3861964"/>
+        <a:ext cx="3132966" cy="986979"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -9197,7 +9133,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9233,7 +9169,7 @@
         <xdr:cNvPr id="4" name="Диаграмма 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9271,7 +9207,7 @@
         <xdr:cNvPr id="6" name="Диаграмма 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9309,7 +9245,7 @@
         <xdr:cNvPr id="7" name="Диаграмма 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9347,7 +9283,7 @@
         <xdr:cNvPr id="5" name="Схема 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9383,7 +9319,7 @@
         <xdr:cNvPr id="8" name="Диаграмма 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9421,7 +9357,7 @@
         <xdr:cNvPr id="9" name="Диаграмма 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9459,7 +9395,7 @@
         <xdr:cNvPr id="10" name="Диаграмма 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9497,7 +9433,7 @@
         <xdr:cNvPr id="11" name="Диаграмма 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9535,7 +9471,7 @@
         <xdr:cNvPr id="12" name="Диаграмма 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9573,7 +9509,7 @@
         <xdr:cNvPr id="13" name="Диаграмма 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9611,7 +9547,7 @@
         <xdr:cNvPr id="14" name="Диаграмма 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9923,7 +9859,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9934,8 +9870,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="B1:W407"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A109" zoomScale="70" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="X134" sqref="X134"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A216" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M193" sqref="M193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10009,51 +9945,51 @@
     <row r="106" spans="7:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="107" spans="7:17" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="K110" s="127"/>
-      <c r="L110" s="127"/>
-      <c r="M110" s="127"/>
-      <c r="N110" s="127"/>
-      <c r="O110" s="127"/>
+      <c r="K110" s="130"/>
+      <c r="L110" s="130"/>
+      <c r="M110" s="130"/>
+      <c r="N110" s="130"/>
+      <c r="O110" s="130"/>
     </row>
     <row r="113" spans="9:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K113" s="127"/>
-      <c r="L113" s="127"/>
-      <c r="M113" s="127"/>
-      <c r="N113" s="127"/>
-      <c r="O113" s="127"/>
+      <c r="K113" s="130"/>
+      <c r="L113" s="130"/>
+      <c r="M113" s="130"/>
+      <c r="N113" s="130"/>
+      <c r="O113" s="130"/>
     </row>
     <row r="116" spans="9:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="K116" s="128"/>
-      <c r="L116" s="128"/>
-      <c r="M116" s="128"/>
-      <c r="N116" s="128"/>
-      <c r="O116" s="128"/>
+      <c r="K116" s="131"/>
+      <c r="L116" s="131"/>
+      <c r="M116" s="131"/>
+      <c r="N116" s="131"/>
+      <c r="O116" s="131"/>
     </row>
     <row r="120" spans="9:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="K120" s="127"/>
-      <c r="L120" s="127"/>
-      <c r="M120" s="127"/>
-      <c r="N120" s="127"/>
-      <c r="O120" s="127"/>
+      <c r="K120" s="130"/>
+      <c r="L120" s="130"/>
+      <c r="M120" s="130"/>
+      <c r="N120" s="130"/>
+      <c r="O120" s="130"/>
     </row>
     <row r="124" spans="9:15" ht="21" x14ac:dyDescent="0.35">
       <c r="I124" s="19"/>
       <c r="J124" s="19"/>
-      <c r="K124" s="126"/>
-      <c r="L124" s="126"/>
-      <c r="M124" s="126"/>
-      <c r="N124" s="126"/>
-      <c r="O124" s="126"/>
+      <c r="K124" s="129"/>
+      <c r="L124" s="129"/>
+      <c r="M124" s="129"/>
+      <c r="N124" s="129"/>
+      <c r="O124" s="129"/>
     </row>
     <row r="127" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="9:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="I128" s="131"/>
-      <c r="J128" s="131"/>
-      <c r="K128" s="131"/>
-      <c r="L128" s="131"/>
-      <c r="M128" s="131"/>
-      <c r="N128" s="131"/>
-      <c r="O128" s="131"/>
+      <c r="I128" s="124"/>
+      <c r="J128" s="124"/>
+      <c r="K128" s="124"/>
+      <c r="L128" s="124"/>
+      <c r="M128" s="124"/>
+      <c r="N128" s="124"/>
+      <c r="O128" s="124"/>
     </row>
     <row r="129" spans="6:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K129" s="16"/>
@@ -10064,31 +10000,31 @@
     <row r="134" spans="6:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="136" spans="6:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="137" spans="6:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F137" s="132" t="s">
+      <c r="F137" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="G137" s="132"/>
-      <c r="H137" s="132" t="s">
+      <c r="G137" s="125"/>
+      <c r="H137" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="I137" s="132"/>
-      <c r="J137" s="132"/>
-      <c r="K137" s="132"/>
-      <c r="L137" s="132" t="s">
+      <c r="I137" s="125"/>
+      <c r="J137" s="125"/>
+      <c r="K137" s="125"/>
+      <c r="L137" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="M137" s="132"/>
+      <c r="M137" s="125"/>
       <c r="N137" s="49"/>
     </row>
     <row r="138" spans="6:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F138" s="125"/>
-      <c r="G138" s="125"/>
-      <c r="H138" s="125"/>
-      <c r="I138" s="125"/>
-      <c r="J138" s="125"/>
-      <c r="K138" s="125"/>
-      <c r="L138" s="125"/>
-      <c r="M138" s="125"/>
+      <c r="F138" s="126"/>
+      <c r="G138" s="126"/>
+      <c r="H138" s="126"/>
+      <c r="I138" s="126"/>
+      <c r="J138" s="126"/>
+      <c r="K138" s="126"/>
+      <c r="L138" s="126"/>
+      <c r="M138" s="126"/>
       <c r="N138" s="50"/>
     </row>
     <row r="139" spans="6:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10114,107 +10050,107 @@
       <c r="N140" s="21"/>
     </row>
     <row r="141" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F141" s="114"/>
-      <c r="G141" s="114"/>
-      <c r="H141" s="125" t="s">
+      <c r="F141" s="132"/>
+      <c r="G141" s="132"/>
+      <c r="H141" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="I141" s="125"/>
-      <c r="J141" s="125"/>
-      <c r="K141" s="125"/>
-      <c r="L141" s="114"/>
-      <c r="M141" s="114"/>
+      <c r="I141" s="126"/>
+      <c r="J141" s="126"/>
+      <c r="K141" s="126"/>
+      <c r="L141" s="132"/>
+      <c r="M141" s="132"/>
       <c r="N141" s="51"/>
     </row>
     <row r="142" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F142" s="115"/>
-      <c r="G142" s="115"/>
-      <c r="H142" s="124" t="s">
+      <c r="F142" s="128"/>
+      <c r="G142" s="128"/>
+      <c r="H142" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="I142" s="124"/>
-      <c r="J142" s="124"/>
-      <c r="K142" s="124"/>
-      <c r="L142" s="115"/>
-      <c r="M142" s="115"/>
+      <c r="I142" s="133"/>
+      <c r="J142" s="133"/>
+      <c r="K142" s="133"/>
+      <c r="L142" s="128"/>
+      <c r="M142" s="128"/>
       <c r="N142" s="51"/>
     </row>
     <row r="143" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F143" s="114"/>
-      <c r="G143" s="114"/>
-      <c r="H143" s="125" t="s">
+      <c r="F143" s="132"/>
+      <c r="G143" s="132"/>
+      <c r="H143" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="I143" s="125"/>
-      <c r="J143" s="125"/>
-      <c r="K143" s="125"/>
-      <c r="L143" s="114"/>
-      <c r="M143" s="114"/>
+      <c r="I143" s="126"/>
+      <c r="J143" s="126"/>
+      <c r="K143" s="126"/>
+      <c r="L143" s="132"/>
+      <c r="M143" s="132"/>
       <c r="N143" s="51"/>
     </row>
     <row r="144" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F144" s="115"/>
-      <c r="G144" s="115"/>
-      <c r="H144" s="124" t="s">
+      <c r="F144" s="128"/>
+      <c r="G144" s="128"/>
+      <c r="H144" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="I144" s="124"/>
-      <c r="J144" s="124"/>
-      <c r="K144" s="124"/>
-      <c r="L144" s="115"/>
-      <c r="M144" s="115"/>
+      <c r="I144" s="133"/>
+      <c r="J144" s="133"/>
+      <c r="K144" s="133"/>
+      <c r="L144" s="128"/>
+      <c r="M144" s="128"/>
       <c r="N144" s="51"/>
     </row>
     <row r="145" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F145" s="114"/>
-      <c r="G145" s="114"/>
-      <c r="H145" s="125" t="s">
+      <c r="F145" s="132"/>
+      <c r="G145" s="132"/>
+      <c r="H145" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="I145" s="125"/>
-      <c r="J145" s="125"/>
-      <c r="K145" s="125"/>
-      <c r="L145" s="114"/>
-      <c r="M145" s="114"/>
+      <c r="I145" s="126"/>
+      <c r="J145" s="126"/>
+      <c r="K145" s="126"/>
+      <c r="L145" s="132"/>
+      <c r="M145" s="132"/>
       <c r="N145" s="51"/>
     </row>
     <row r="146" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F146" s="115"/>
-      <c r="G146" s="115"/>
-      <c r="H146" s="124" t="s">
+      <c r="F146" s="128"/>
+      <c r="G146" s="128"/>
+      <c r="H146" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="I146" s="124"/>
-      <c r="J146" s="124"/>
-      <c r="K146" s="124"/>
-      <c r="L146" s="115"/>
-      <c r="M146" s="115"/>
+      <c r="I146" s="133"/>
+      <c r="J146" s="133"/>
+      <c r="K146" s="133"/>
+      <c r="L146" s="128"/>
+      <c r="M146" s="128"/>
       <c r="N146" s="51"/>
     </row>
     <row r="147" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F147" s="114"/>
-      <c r="G147" s="114"/>
-      <c r="H147" s="125" t="s">
+      <c r="F147" s="132"/>
+      <c r="G147" s="132"/>
+      <c r="H147" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="I147" s="125"/>
-      <c r="J147" s="125"/>
-      <c r="K147" s="125"/>
-      <c r="L147" s="114"/>
-      <c r="M147" s="114"/>
+      <c r="I147" s="126"/>
+      <c r="J147" s="126"/>
+      <c r="K147" s="126"/>
+      <c r="L147" s="132"/>
+      <c r="M147" s="132"/>
       <c r="N147" s="51"/>
     </row>
     <row r="148" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F148" s="115"/>
-      <c r="G148" s="115"/>
-      <c r="H148" s="124" t="s">
+      <c r="F148" s="128"/>
+      <c r="G148" s="128"/>
+      <c r="H148" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="I148" s="124"/>
-      <c r="J148" s="124"/>
-      <c r="K148" s="124"/>
-      <c r="L148" s="115"/>
-      <c r="M148" s="115"/>
+      <c r="I148" s="133"/>
+      <c r="J148" s="133"/>
+      <c r="K148" s="133"/>
+      <c r="L148" s="128"/>
+      <c r="M148" s="128"/>
       <c r="N148" s="51"/>
     </row>
     <row r="162" spans="5:23" ht="23.25" x14ac:dyDescent="0.25">
@@ -10247,20 +10183,20 @@
       <c r="J191" s="23"/>
       <c r="K191" s="23"/>
       <c r="L191" s="23"/>
-      <c r="M191" s="116"/>
-      <c r="N191" s="116"/>
-      <c r="O191" s="116"/>
-      <c r="P191" s="116"/>
+      <c r="M191" s="23"/>
+      <c r="N191" s="23"/>
+      <c r="O191" s="23"/>
+      <c r="P191" s="23"/>
     </row>
     <row r="192" spans="5:16" ht="21" x14ac:dyDescent="0.35">
       <c r="E192" s="23"/>
       <c r="J192" s="23"/>
       <c r="K192" s="23"/>
       <c r="L192" s="23"/>
-      <c r="M192" s="116"/>
-      <c r="N192" s="116"/>
-      <c r="O192" s="116"/>
-      <c r="P192" s="116"/>
+      <c r="M192" s="23"/>
+      <c r="N192" s="23"/>
+      <c r="O192" s="23"/>
+      <c r="P192" s="23"/>
     </row>
     <row r="195" spans="2:23" ht="21" x14ac:dyDescent="0.35">
       <c r="B195" s="23"/>
@@ -10291,26 +10227,26 @@
       </c>
     </row>
     <row r="203" spans="2:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="D203" s="134" t="s">
+      <c r="D203" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="E203" s="134"/>
-      <c r="F203" s="134"/>
-      <c r="G203" s="135"/>
-      <c r="H203" s="136" t="s">
+      <c r="E203" s="112"/>
+      <c r="F203" s="112"/>
+      <c r="G203" s="113"/>
+      <c r="H203" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="I203" s="134"/>
-      <c r="J203" s="134"/>
-      <c r="K203" s="137"/>
-      <c r="L203" s="138" t="s">
+      <c r="I203" s="112"/>
+      <c r="J203" s="112"/>
+      <c r="K203" s="115"/>
+      <c r="L203" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="M203" s="134"/>
-      <c r="N203" s="134"/>
-      <c r="O203" s="134"/>
-      <c r="P203" s="134"/>
-      <c r="Q203" s="137"/>
+      <c r="M203" s="112"/>
+      <c r="N203" s="112"/>
+      <c r="O203" s="112"/>
+      <c r="P203" s="112"/>
+      <c r="Q203" s="115"/>
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E204" s="26"/>
@@ -10401,18 +10337,18 @@
         <v>41</v>
       </c>
       <c r="E211" s="110"/>
-      <c r="F211" s="133"/>
-      <c r="G211" s="133"/>
+      <c r="F211" s="120"/>
+      <c r="G211" s="120"/>
       <c r="H211" s="53"/>
-      <c r="I211" s="133"/>
-      <c r="J211" s="133"/>
-      <c r="K211" s="133"/>
+      <c r="I211" s="120"/>
+      <c r="J211" s="120"/>
+      <c r="K211" s="120"/>
       <c r="L211" s="60"/>
       <c r="M211" s="53"/>
       <c r="N211" s="53"/>
-      <c r="O211" s="133"/>
-      <c r="P211" s="133"/>
-      <c r="Q211" s="133"/>
+      <c r="O211" s="120"/>
+      <c r="P211" s="120"/>
+      <c r="Q211" s="120"/>
     </row>
     <row r="212" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B212" s="52"/>
@@ -10421,36 +10357,36 @@
         <v>42</v>
       </c>
       <c r="E212" s="111"/>
-      <c r="F212" s="139"/>
-      <c r="G212" s="139"/>
+      <c r="F212" s="119"/>
+      <c r="G212" s="119"/>
       <c r="H212" s="54"/>
-      <c r="I212" s="139"/>
-      <c r="J212" s="139"/>
-      <c r="K212" s="139"/>
+      <c r="I212" s="119"/>
+      <c r="J212" s="119"/>
+      <c r="K212" s="119"/>
       <c r="L212" s="61"/>
       <c r="M212" s="54"/>
       <c r="N212" s="54"/>
-      <c r="O212" s="139"/>
-      <c r="P212" s="139"/>
-      <c r="Q212" s="139"/>
+      <c r="O212" s="119"/>
+      <c r="P212" s="119"/>
+      <c r="Q212" s="119"/>
     </row>
     <row r="213" spans="2:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D213" s="55" t="s">
         <v>43</v>
       </c>
       <c r="E213" s="110"/>
-      <c r="F213" s="133"/>
-      <c r="G213" s="133"/>
+      <c r="F213" s="120"/>
+      <c r="G213" s="120"/>
       <c r="H213" s="53"/>
-      <c r="I213" s="133"/>
-      <c r="J213" s="133"/>
-      <c r="K213" s="133"/>
+      <c r="I213" s="120"/>
+      <c r="J213" s="120"/>
+      <c r="K213" s="120"/>
       <c r="L213" s="60"/>
       <c r="M213" s="53"/>
       <c r="N213" s="53"/>
-      <c r="O213" s="133"/>
-      <c r="P213" s="133"/>
-      <c r="Q213" s="133"/>
+      <c r="O213" s="120"/>
+      <c r="P213" s="120"/>
+      <c r="Q213" s="120"/>
     </row>
     <row r="215" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
@@ -10499,17 +10435,17 @@
       <c r="N263" s="24"/>
     </row>
     <row r="266" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B266" s="116" t="s">
+      <c r="B266" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="C266" s="116"/>
-      <c r="D266" s="116"/>
+      <c r="C266" s="127"/>
+      <c r="D266" s="127"/>
       <c r="E266" s="44"/>
       <c r="F266" s="44"/>
-      <c r="G266" s="116" t="s">
+      <c r="G266" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="H266" s="116"/>
+      <c r="H266" s="127"/>
     </row>
     <row r="267" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E267" s="36"/>
@@ -10548,23 +10484,23 @@
       <c r="E278" s="36"/>
     </row>
     <row r="279" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B279" s="118" t="s">
+      <c r="B279" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="C279" s="118"/>
-      <c r="D279" s="118"/>
+      <c r="C279" s="139"/>
+      <c r="D279" s="139"/>
       <c r="E279" s="36"/>
-      <c r="G279" s="118" t="s">
+      <c r="G279" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="H279" s="118"/>
+      <c r="H279" s="139"/>
     </row>
     <row r="280" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B280" s="117"/>
-      <c r="C280" s="117"/>
-      <c r="D280" s="117"/>
-      <c r="G280" s="117"/>
-      <c r="H280" s="117"/>
+      <c r="B280" s="138"/>
+      <c r="C280" s="138"/>
+      <c r="D280" s="138"/>
+      <c r="G280" s="138"/>
+      <c r="H280" s="138"/>
     </row>
     <row r="282" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C282" s="25"/>
@@ -10667,76 +10603,76 @@
     <row r="367" spans="4:15" ht="7.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="368" spans="4:15" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="370" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B370" s="119" t="s">
+      <c r="B370" s="122" t="s">
         <v>72</v>
       </c>
-      <c r="C370" s="119"/>
-      <c r="D370" s="119"/>
-      <c r="E370" s="119"/>
-      <c r="F370" s="119"/>
-      <c r="G370" s="119"/>
-      <c r="H370" s="120"/>
-      <c r="I370" s="120"/>
+      <c r="C370" s="122"/>
+      <c r="D370" s="122"/>
+      <c r="E370" s="122"/>
+      <c r="F370" s="122"/>
+      <c r="G370" s="122"/>
+      <c r="H370" s="134"/>
+      <c r="I370" s="134"/>
     </row>
     <row r="371" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B371" s="122" t="s">
+      <c r="B371" s="136" t="s">
         <v>73</v>
       </c>
-      <c r="C371" s="122"/>
-      <c r="D371" s="122"/>
-      <c r="E371" s="122"/>
-      <c r="F371" s="122"/>
-      <c r="G371" s="122"/>
-      <c r="H371" s="121"/>
-      <c r="I371" s="121"/>
+      <c r="C371" s="136"/>
+      <c r="D371" s="136"/>
+      <c r="E371" s="136"/>
+      <c r="F371" s="136"/>
+      <c r="G371" s="136"/>
+      <c r="H371" s="135"/>
+      <c r="I371" s="135"/>
     </row>
     <row r="372" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B372" s="123" t="s">
+      <c r="B372" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="C372" s="123"/>
-      <c r="D372" s="123"/>
-      <c r="E372" s="123"/>
-      <c r="F372" s="123"/>
-      <c r="G372" s="123"/>
-      <c r="H372" s="120"/>
-      <c r="I372" s="120"/>
+      <c r="C372" s="137"/>
+      <c r="D372" s="137"/>
+      <c r="E372" s="137"/>
+      <c r="F372" s="137"/>
+      <c r="G372" s="137"/>
+      <c r="H372" s="134"/>
+      <c r="I372" s="134"/>
     </row>
     <row r="376" spans="2:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K376" s="119" t="s">
+      <c r="K376" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="L376" s="119"/>
-      <c r="M376" s="119"/>
-      <c r="N376" s="119"/>
-      <c r="O376" s="119"/>
-      <c r="P376" s="141"/>
-      <c r="Q376" s="141"/>
-      <c r="R376" s="141"/>
+      <c r="L376" s="122"/>
+      <c r="M376" s="122"/>
+      <c r="N376" s="122"/>
+      <c r="O376" s="122"/>
+      <c r="P376" s="123"/>
+      <c r="Q376" s="123"/>
+      <c r="R376" s="123"/>
     </row>
     <row r="377" spans="2:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K377" s="140" t="s">
+      <c r="K377" s="121" t="s">
         <v>96</v>
       </c>
-      <c r="L377" s="140"/>
-      <c r="M377" s="140"/>
-      <c r="N377" s="140"/>
-      <c r="O377" s="140"/>
-      <c r="P377" s="112"/>
-      <c r="Q377" s="112"/>
-      <c r="R377" s="112"/>
+      <c r="L377" s="121"/>
+      <c r="M377" s="121"/>
+      <c r="N377" s="121"/>
+      <c r="O377" s="121"/>
+      <c r="P377" s="140"/>
+      <c r="Q377" s="140"/>
+      <c r="R377" s="140"/>
     </row>
     <row r="378" spans="2:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K378" s="119" t="s">
+      <c r="K378" s="122" t="s">
         <v>95</v>
       </c>
-      <c r="L378" s="119"/>
-      <c r="M378" s="119"/>
-      <c r="N378" s="119"/>
-      <c r="O378" s="119"/>
-      <c r="P378" s="113"/>
-      <c r="Q378" s="113"/>
-      <c r="R378" s="113"/>
+      <c r="L378" s="122"/>
+      <c r="M378" s="122"/>
+      <c r="N378" s="122"/>
+      <c r="O378" s="122"/>
+      <c r="P378" s="141"/>
+      <c r="Q378" s="141"/>
+      <c r="R378" s="141"/>
     </row>
     <row r="388" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H388" s="63" t="s">
@@ -10750,43 +10686,43 @@
       <c r="N388" s="40"/>
     </row>
     <row r="391" spans="2:20" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B391" s="130" t="s">
+      <c r="B391" s="117" t="s">
         <v>84</v>
       </c>
-      <c r="C391" s="130"/>
-      <c r="D391" s="130"/>
-      <c r="E391" s="130"/>
-      <c r="F391" s="130" t="s">
+      <c r="C391" s="117"/>
+      <c r="D391" s="117"/>
+      <c r="E391" s="117"/>
+      <c r="F391" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="G391" s="130"/>
-      <c r="H391" s="130"/>
-      <c r="I391" s="130" t="s">
+      <c r="G391" s="117"/>
+      <c r="H391" s="117"/>
+      <c r="I391" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="J391" s="130"/>
+      <c r="J391" s="117"/>
       <c r="K391" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="L391" s="129" t="s">
+      <c r="L391" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="M391" s="129"/>
-      <c r="N391" s="129" t="s">
+      <c r="M391" s="118"/>
+      <c r="N391" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="O391" s="129"/>
-      <c r="P391" s="130" t="s">
+      <c r="O391" s="118"/>
+      <c r="P391" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="Q391" s="130"/>
+      <c r="Q391" s="117"/>
       <c r="R391" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="S391" s="129" t="s">
+      <c r="S391" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="T391" s="129"/>
+      <c r="T391" s="118"/>
     </row>
     <row r="392" spans="2:20" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B392" s="72"/>
@@ -11125,7 +11061,64 @@
       <c r="T407" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="73">
+    <mergeCell ref="P377:R377"/>
+    <mergeCell ref="P378:R378"/>
+    <mergeCell ref="L141:M141"/>
+    <mergeCell ref="L142:M142"/>
+    <mergeCell ref="L143:M143"/>
+    <mergeCell ref="L144:M144"/>
+    <mergeCell ref="L145:M145"/>
+    <mergeCell ref="L147:M147"/>
+    <mergeCell ref="L148:M148"/>
+    <mergeCell ref="K376:O376"/>
+    <mergeCell ref="B266:D266"/>
+    <mergeCell ref="G266:H266"/>
+    <mergeCell ref="B280:D280"/>
+    <mergeCell ref="G280:H280"/>
+    <mergeCell ref="B279:D279"/>
+    <mergeCell ref="G279:H279"/>
+    <mergeCell ref="H370:I370"/>
+    <mergeCell ref="H371:I371"/>
+    <mergeCell ref="H372:I372"/>
+    <mergeCell ref="B370:G370"/>
+    <mergeCell ref="B371:G371"/>
+    <mergeCell ref="B372:G372"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="F142:G142"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="F146:G146"/>
+    <mergeCell ref="F147:G147"/>
+    <mergeCell ref="F148:G148"/>
+    <mergeCell ref="F145:G145"/>
+    <mergeCell ref="F143:G143"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="K124:O124"/>
+    <mergeCell ref="K110:O110"/>
+    <mergeCell ref="K116:O116"/>
+    <mergeCell ref="K113:O113"/>
+    <mergeCell ref="K120:O120"/>
+    <mergeCell ref="S391:T391"/>
+    <mergeCell ref="I391:J391"/>
+    <mergeCell ref="P391:Q391"/>
+    <mergeCell ref="I128:O128"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="F138:G138"/>
+    <mergeCell ref="H138:K138"/>
+    <mergeCell ref="L137:M137"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="L138:M138"/>
+    <mergeCell ref="F211:G211"/>
+    <mergeCell ref="I211:K211"/>
+    <mergeCell ref="O211:Q211"/>
+    <mergeCell ref="L146:M146"/>
     <mergeCell ref="D203:G203"/>
     <mergeCell ref="H203:K203"/>
     <mergeCell ref="L203:Q203"/>
@@ -11142,65 +11135,6 @@
     <mergeCell ref="K377:O377"/>
     <mergeCell ref="K378:O378"/>
     <mergeCell ref="P376:R376"/>
-    <mergeCell ref="S391:T391"/>
-    <mergeCell ref="I391:J391"/>
-    <mergeCell ref="P391:Q391"/>
-    <mergeCell ref="I128:O128"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="F138:G138"/>
-    <mergeCell ref="H138:K138"/>
-    <mergeCell ref="L137:M137"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="L138:M138"/>
-    <mergeCell ref="F211:G211"/>
-    <mergeCell ref="I211:K211"/>
-    <mergeCell ref="O211:Q211"/>
-    <mergeCell ref="M192:P192"/>
-    <mergeCell ref="M191:P191"/>
-    <mergeCell ref="L146:M146"/>
-    <mergeCell ref="K124:O124"/>
-    <mergeCell ref="K110:O110"/>
-    <mergeCell ref="K116:O116"/>
-    <mergeCell ref="K113:O113"/>
-    <mergeCell ref="K120:O120"/>
-    <mergeCell ref="F141:G141"/>
-    <mergeCell ref="F142:G142"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="F146:G146"/>
-    <mergeCell ref="F147:G147"/>
-    <mergeCell ref="F148:G148"/>
-    <mergeCell ref="F145:G145"/>
-    <mergeCell ref="F143:G143"/>
-    <mergeCell ref="F144:G144"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
-    <mergeCell ref="H370:I370"/>
-    <mergeCell ref="H371:I371"/>
-    <mergeCell ref="H372:I372"/>
-    <mergeCell ref="B370:G370"/>
-    <mergeCell ref="B371:G371"/>
-    <mergeCell ref="B372:G372"/>
-    <mergeCell ref="B266:D266"/>
-    <mergeCell ref="G266:H266"/>
-    <mergeCell ref="B280:D280"/>
-    <mergeCell ref="G280:H280"/>
-    <mergeCell ref="B279:D279"/>
-    <mergeCell ref="G279:H279"/>
-    <mergeCell ref="P377:R377"/>
-    <mergeCell ref="P378:R378"/>
-    <mergeCell ref="L141:M141"/>
-    <mergeCell ref="L142:M142"/>
-    <mergeCell ref="L143:M143"/>
-    <mergeCell ref="L144:M144"/>
-    <mergeCell ref="L145:M145"/>
-    <mergeCell ref="L147:M147"/>
-    <mergeCell ref="L148:M148"/>
-    <mergeCell ref="K376:O376"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
@@ -11214,7 +11148,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+      <selection activeCell="E2" sqref="E2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11324,39 +11258,53 @@
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="14"/>
       <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="14"/>
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
+      <c r="E4"/>
+      <c r="F4"/>
       <c r="G4" s="14"/>
       <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
+      <c r="E5"/>
+      <c r="F5"/>
       <c r="G5" s="14"/>
       <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
+      <c r="E6"/>
+      <c r="F6"/>
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
+      <c r="E7"/>
+      <c r="F7"/>
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
+      <c r="E8"/>
+      <c r="F8"/>
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -11556,262 +11504,297 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155" t="s">
+      <c r="B24" s="145"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="155"/>
-      <c r="G24" s="155"/>
-      <c r="H24" s="155" t="s">
+      <c r="F24" s="145"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="155"/>
+      <c r="I24" s="145"/>
       <c r="J24" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="K24" s="152" t="s">
+      <c r="K24" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="L24" s="152"/>
-      <c r="M24" s="152" t="s">
+      <c r="L24" s="142"/>
+      <c r="M24" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="N24" s="152"/>
-      <c r="O24" s="155" t="s">
+      <c r="N24" s="142"/>
+      <c r="O24" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="P24" s="155"/>
+      <c r="P24" s="145"/>
       <c r="Q24" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="R24" s="152" t="s">
+      <c r="R24" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="S24" s="152"/>
+      <c r="S24" s="142"/>
     </row>
     <row r="25" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="153" t="s">
+      <c r="A25" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="153"/>
-      <c r="C25" s="153"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="153" t="s">
+      <c r="B25" s="143"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="143"/>
+      <c r="E25" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="153"/>
-      <c r="G25" s="153"/>
-      <c r="H25" s="153" t="s">
+      <c r="F25" s="143"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="153"/>
+      <c r="I25" s="143"/>
       <c r="J25" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="K25" s="154" t="s">
+      <c r="K25" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="L25" s="154"/>
-      <c r="M25" s="154" t="s">
+      <c r="L25" s="144"/>
+      <c r="M25" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="N25" s="154"/>
-      <c r="O25" s="153" t="s">
+      <c r="N25" s="144"/>
+      <c r="O25" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="P25" s="153"/>
+      <c r="P25" s="143"/>
       <c r="Q25" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="R25" s="154" t="s">
+      <c r="R25" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="S25" s="154"/>
+      <c r="S25" s="144"/>
     </row>
     <row r="26" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="151" t="s">
+      <c r="A26" s="149" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="151"/>
-      <c r="C26" s="151"/>
-      <c r="D26" s="151"/>
-      <c r="E26" s="151" t="s">
+      <c r="B26" s="149"/>
+      <c r="C26" s="149"/>
+      <c r="D26" s="149"/>
+      <c r="E26" s="149" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="151"/>
-      <c r="G26" s="151"/>
-      <c r="H26" s="151" t="s">
+      <c r="F26" s="149"/>
+      <c r="G26" s="149"/>
+      <c r="H26" s="149" t="s">
         <v>91</v>
       </c>
-      <c r="I26" s="151"/>
+      <c r="I26" s="149"/>
       <c r="J26" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="148" t="s">
+      <c r="K26" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="L26" s="148"/>
-      <c r="M26" s="148" t="s">
+      <c r="L26" s="146"/>
+      <c r="M26" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="N26" s="148"/>
-      <c r="O26" s="151" t="s">
+      <c r="N26" s="146"/>
+      <c r="O26" s="149" t="s">
         <v>91</v>
       </c>
-      <c r="P26" s="151"/>
+      <c r="P26" s="149"/>
       <c r="Q26" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="R26" s="148" t="s">
+      <c r="R26" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="S26" s="148"/>
+      <c r="S26" s="146"/>
     </row>
     <row r="27" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="149" t="s">
+      <c r="A27" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="149"/>
-      <c r="C27" s="149"/>
-      <c r="D27" s="149"/>
-      <c r="E27" s="149" t="s">
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="149"/>
-      <c r="G27" s="149"/>
-      <c r="H27" s="149" t="s">
+      <c r="F27" s="147"/>
+      <c r="G27" s="147"/>
+      <c r="H27" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="149"/>
+      <c r="I27" s="147"/>
       <c r="J27" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="K27" s="150" t="s">
+      <c r="K27" s="148" t="s">
         <v>91</v>
       </c>
-      <c r="L27" s="150"/>
-      <c r="M27" s="150" t="s">
+      <c r="L27" s="148"/>
+      <c r="M27" s="148" t="s">
         <v>91</v>
       </c>
-      <c r="N27" s="150"/>
-      <c r="O27" s="149" t="s">
+      <c r="N27" s="148"/>
+      <c r="O27" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="P27" s="149"/>
+      <c r="P27" s="147"/>
       <c r="Q27" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="R27" s="150" t="s">
+      <c r="R27" s="148" t="s">
         <v>91</v>
       </c>
-      <c r="S27" s="150"/>
+      <c r="S27" s="148"/>
     </row>
     <row r="28" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="147" t="s">
+      <c r="A28" s="153" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="147"/>
-      <c r="C28" s="147"/>
-      <c r="D28" s="147"/>
-      <c r="E28" s="147" t="s">
+      <c r="B28" s="153"/>
+      <c r="C28" s="153"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="153" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="147"/>
-      <c r="G28" s="147"/>
-      <c r="H28" s="147" t="s">
+      <c r="F28" s="153"/>
+      <c r="G28" s="153"/>
+      <c r="H28" s="153" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="147"/>
+      <c r="I28" s="153"/>
       <c r="J28" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="K28" s="144" t="s">
+      <c r="K28" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="L28" s="144"/>
-      <c r="M28" s="144" t="s">
+      <c r="L28" s="150"/>
+      <c r="M28" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="N28" s="144"/>
-      <c r="O28" s="147" t="s">
+      <c r="N28" s="150"/>
+      <c r="O28" s="153" t="s">
         <v>91</v>
       </c>
-      <c r="P28" s="147"/>
+      <c r="P28" s="153"/>
       <c r="Q28" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="R28" s="144" t="s">
+      <c r="R28" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="S28" s="144"/>
+      <c r="S28" s="150"/>
     </row>
     <row r="29" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="145" t="s">
+      <c r="A29" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="145"/>
-      <c r="C29" s="145"/>
-      <c r="D29" s="145"/>
-      <c r="E29" s="145" t="s">
+      <c r="B29" s="151"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="151"/>
+      <c r="E29" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="145"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="145" t="s">
+      <c r="F29" s="151"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="145"/>
+      <c r="I29" s="151"/>
       <c r="J29" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="K29" s="146" t="s">
+      <c r="K29" s="152" t="s">
         <v>91</v>
       </c>
-      <c r="L29" s="146"/>
-      <c r="M29" s="146" t="s">
+      <c r="L29" s="152"/>
+      <c r="M29" s="152" t="s">
         <v>91</v>
       </c>
-      <c r="N29" s="146"/>
-      <c r="O29" s="145" t="s">
+      <c r="N29" s="152"/>
+      <c r="O29" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="P29" s="145"/>
+      <c r="P29" s="151"/>
       <c r="Q29" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="R29" s="146" t="s">
+      <c r="R29" s="152" t="s">
         <v>91</v>
       </c>
-      <c r="S29" s="146"/>
+      <c r="S29" s="152"/>
     </row>
     <row r="30" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="143"/>
-      <c r="B30" s="143"/>
-      <c r="C30" s="143"/>
-      <c r="D30" s="143"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="143"/>
+      <c r="A30" s="155"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="155"/>
+      <c r="H30" s="155"/>
+      <c r="I30" s="155"/>
       <c r="J30" s="65"/>
-      <c r="K30" s="142"/>
-      <c r="L30" s="142"/>
-      <c r="M30" s="142"/>
-      <c r="N30" s="142"/>
-      <c r="O30" s="143"/>
-      <c r="P30" s="143"/>
+      <c r="K30" s="154"/>
+      <c r="L30" s="154"/>
+      <c r="M30" s="154"/>
+      <c r="N30" s="154"/>
+      <c r="O30" s="155"/>
+      <c r="P30" s="155"/>
       <c r="Q30" s="64"/>
-      <c r="R30" s="142"/>
-      <c r="S30" s="142"/>
+      <c r="R30" s="154"/>
+      <c r="S30" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
     <mergeCell ref="R24:S24"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="E25:G25"/>
@@ -11826,41 +11809,6 @@
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="O24:P24"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="O30:P30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add recommendation to other sheet
</commit_message>
<xml_diff>
--- a/template/Report.xlsx
+++ b/template/Report.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\analytics\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liubava\Documents\GitHub\analytics\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="2" r:id="rId1"/>
-    <sheet name="ChanelTrafic" sheetId="1" state="hidden" r:id="rId2"/>
-    <sheet name="style" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="recommendation" sheetId="6" r:id="rId2"/>
+    <sheet name="ChanelTrafic" sheetId="1" state="hidden" r:id="rId3"/>
+    <sheet name="style" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ad">report!$F$384</definedName>
@@ -133,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
   <si>
     <t>quality</t>
   </si>
@@ -371,16 +372,19 @@
   <si>
     <t>Количество обращений</t>
   </si>
+  <si>
+    <t>Рекомендации Заголовок</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00&quot;р.&quot;"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00&quot;р.&quot;"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -509,13 +513,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri Light"/>
@@ -539,8 +536,16 @@
       <charset val="204"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,12 +643,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -722,12 +721,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -751,7 +750,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -792,17 +791,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -835,210 +827,97 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="15" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="15" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="15" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="15" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="15" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="15" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="16" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="16" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="16" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="16" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="16" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="16" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="10" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1056,56 +935,131 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1137,7 +1091,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1255,7 +1209,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1296,7 +1250,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1337,7 +1291,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1378,7 +1332,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1419,7 +1373,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1460,7 +1414,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1513,7 +1467,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -1535,7 +1489,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
             </c:ext>
@@ -1631,7 +1585,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1673,7 +1627,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1688,7 +1642,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1716,7 +1670,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1731,7 +1685,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1759,7 +1713,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1774,7 +1728,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1789,11 +1743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="119889920"/>
-        <c:axId val="119891456"/>
+        <c:axId val="254704304"/>
+        <c:axId val="254703912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="119889920"/>
+        <c:axId val="254704304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1802,7 +1756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119891456"/>
+        <c:crossAx val="254703912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1810,7 +1764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119891456"/>
+        <c:axId val="254703912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,7 +1785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119889920"/>
+        <c:crossAx val="254704304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1880,7 +1834,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1922,7 +1876,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1940,12 +1894,12 @@
             <c:numRef>
               <c:f>[0]!sendall2</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\ ##0.00"р."_-;\-* #\ ##0.00"р."_-;_-* "-"??"р."_-;_-@_-</c:formatCode>
+                <c:formatCode>_("р."* #,##0.00_);_("р."* \(#,##0.00\);_("р."* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -1973,7 +1927,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1991,12 +1945,12 @@
             <c:numRef>
               <c:f>[0]!costConversation</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\ ##0.00"р."_-;\-* #\ ##0.00"р."_-;_-* "-"??"р."_-;_-@_-</c:formatCode>
+                <c:formatCode>_("р."* #,##0.00_);_("р."* \(#,##0.00\);_("р."* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2024,7 +1978,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2047,7 +2001,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2062,11 +2016,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="126325888"/>
-        <c:axId val="126327424"/>
+        <c:axId val="254705872"/>
+        <c:axId val="254706264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126325888"/>
+        <c:axId val="254705872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,7 +2030,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126327424"/>
+        <c:crossAx val="254706264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2084,23 +2038,24 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126327424"/>
+        <c:axId val="254706264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="_-* #\ ##0.00&quot;р.&quot;_-;\-* #\ ##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-" sourceLinked="1"/>
+        <c:numFmt formatCode="_(&quot;р.&quot;* #,##0.00_);_(&quot;р.&quot;* \(#,##0.00\);_(&quot;р.&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126325888"/>
+        <c:crossAx val="254705872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2133,7 +2088,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2194,7 +2149,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1FE8-4CC8-A3E6-CD574745982A}"/>
             </c:ext>
@@ -2209,11 +2164,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="140464128"/>
-        <c:axId val="140465664"/>
+        <c:axId val="252456576"/>
+        <c:axId val="252427736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="140464128"/>
+        <c:axId val="252456576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2211,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140465664"/>
+        <c:crossAx val="252427736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2264,7 +2219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140465664"/>
+        <c:axId val="252427736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2310,7 +2265,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140464128"/>
+        <c:crossAx val="252456576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2355,7 +2310,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2394,7 +2349,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-5B18-40B8-9E6F-B2250215750F}"/>
               </c:ext>
@@ -2414,7 +2369,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-5B18-40B8-9E6F-B2250215750F}"/>
               </c:ext>
@@ -2471,7 +2426,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -2493,7 +2448,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-5B18-40B8-9E6F-B2250215750F}"/>
             </c:ext>
@@ -2592,7 +2547,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2646,7 +2601,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6DCE-4170-A8BA-4BE124766687}"/>
             </c:ext>
@@ -2705,7 +2660,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -2758,7 +2713,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6DCE-4170-A8BA-4BE124766687}"/>
             </c:ext>
@@ -2774,11 +2729,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="97890688"/>
-        <c:axId val="97892224"/>
+        <c:axId val="253154224"/>
+        <c:axId val="253154608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97890688"/>
+        <c:axId val="253154224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2821,7 +2776,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97892224"/>
+        <c:crossAx val="253154608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2829,7 +2784,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97892224"/>
+        <c:axId val="253154608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2880,7 +2835,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97890688"/>
+        <c:crossAx val="253154224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2894,6 +2849,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2956,7 +2912,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2993,7 +2949,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3015,7 +2971,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9533-424E-9DFF-B9454BE51E98}"/>
             </c:ext>
@@ -3035,6 +2991,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3067,7 +3024,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3119,7 +3076,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3143,7 +3100,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1C8B-4851-BE55-E5C0FF949603}"/>
             </c:ext>
@@ -3181,7 +3138,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3205,7 +3162,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1C8B-4851-BE55-E5C0FF949603}"/>
             </c:ext>
@@ -3220,11 +3177,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102066816"/>
-        <c:axId val="102068608"/>
+        <c:axId val="254534152"/>
+        <c:axId val="214086992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102066816"/>
+        <c:axId val="254534152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3234,7 +3191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102068608"/>
+        <c:crossAx val="214086992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3242,7 +3199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102068608"/>
+        <c:axId val="214086992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3253,13 +3210,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102066816"/>
+        <c:crossAx val="254534152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3280,7 +3238,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3311,6 +3269,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3335,7 +3294,7 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:explosion val="6"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-1576-4393-8E4F-7B3A075ADDFE}"/>
               </c:ext>
@@ -3356,7 +3315,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3378,7 +3337,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1576-4393-8E4F-7B3A075ADDFE}"/>
             </c:ext>
@@ -3414,7 +3373,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3457,7 +3416,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3EA3-48D1-8E98-DC97D53A6E0F}"/>
             </c:ext>
@@ -3487,7 +3446,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3EA3-48D1-8E98-DC97D53A6E0F}"/>
             </c:ext>
@@ -3501,11 +3460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119812480"/>
-        <c:axId val="119814016"/>
+        <c:axId val="214085424"/>
+        <c:axId val="214087384"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="119812480"/>
+        <c:axId val="214085424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3515,7 +3474,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119814016"/>
+        <c:crossAx val="214087384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3523,7 +3482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119814016"/>
+        <c:axId val="214087384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3534,13 +3493,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119812480"/>
+        <c:crossAx val="214085424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3573,7 +3533,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3616,7 +3576,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5324-4B7B-AB47-40E0FE10B1A4}"/>
             </c:ext>
@@ -3646,7 +3606,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5324-4B7B-AB47-40E0FE10B1A4}"/>
             </c:ext>
@@ -3660,11 +3620,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119827840"/>
-        <c:axId val="119837824"/>
+        <c:axId val="254705088"/>
+        <c:axId val="254705480"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="119827840"/>
+        <c:axId val="254705088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3674,7 +3634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119837824"/>
+        <c:crossAx val="254705480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3682,7 +3642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119837824"/>
+        <c:axId val="254705480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3693,13 +3653,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119827840"/>
+        <c:crossAx val="254705088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -7083,6 +7044,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AFF118AE-0192-452D-9AB7-AD9749DBEBF5}" type="pres">
       <dgm:prSet presAssocID="{D0B5C048-8C24-4F76-8C9D-7762D594F997}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7092,6 +7060,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{79388EF3-A8BE-4117-ACBA-8A08FF47472A}" type="pres">
       <dgm:prSet presAssocID="{A43066EC-58A2-4A7D-AF6B-37D46EA26464}" presName="Name8" presStyleCnt="0"/>
@@ -7105,6 +7080,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{673D1501-484B-4334-879E-3653F69F415A}" type="pres">
       <dgm:prSet presAssocID="{A43066EC-58A2-4A7D-AF6B-37D46EA26464}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7114,6 +7096,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{47D67E14-1695-4B93-9EB1-4CC623CC53C2}" type="pres">
       <dgm:prSet presAssocID="{93154AA3-294E-4A72-A452-A70CA494AC1C}" presName="Name8" presStyleCnt="0"/>
@@ -7127,6 +7116,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{E32FEE9D-FC56-4633-B235-BB4BC8FB2096}" type="pres">
       <dgm:prSet presAssocID="{93154AA3-294E-4A72-A452-A70CA494AC1C}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7136,6 +7132,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8AAD1D77-9DFF-4406-995B-9E373EE560D6}" type="pres">
       <dgm:prSet presAssocID="{6F6CEB40-F018-40B7-B43C-BB0F608C1737}" presName="Name8" presStyleCnt="0"/>
@@ -7149,6 +7152,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{166B6DC3-E48C-470D-B319-D777F3D4DA8C}" type="pres">
       <dgm:prSet presAssocID="{6F6CEB40-F018-40B7-B43C-BB0F608C1737}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7158,6 +7168,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7A3E38AC-ABE0-44B1-ABFE-C71AA69B5E79}" type="pres">
       <dgm:prSet presAssocID="{DFB816DE-9FE1-4A03-BBE3-E92EDD0106A3}" presName="Name8" presStyleCnt="0"/>
@@ -7171,6 +7188,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{53E7FBCA-B0EF-4CD3-9E52-80F3A839A7EA}" type="pres">
       <dgm:prSet presAssocID="{DFB816DE-9FE1-4A03-BBE3-E92EDD0106A3}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7180,6 +7204,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{40A0CFF3-5D9A-46B0-B3E9-C705D72172EE}" type="pres">
       <dgm:prSet presAssocID="{9672259E-8D62-4911-A026-2E23FD52D48A}" presName="Name8" presStyleCnt="0"/>
@@ -7193,6 +7224,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{22C6AEA5-B4B3-41C7-AE03-AA0A4D4EB3BF}" type="pres">
       <dgm:prSet presAssocID="{9672259E-8D62-4911-A026-2E23FD52D48A}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7202,6 +7240,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
@@ -7319,7 +7364,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7329,7 +7374,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7407,7 +7451,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7417,7 +7461,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7495,7 +7538,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7505,7 +7548,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7583,7 +7625,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7593,7 +7635,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7671,7 +7712,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7681,7 +7722,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7756,7 +7796,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7766,7 +7806,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="2000" kern="1200">
@@ -9083,7 +9122,7 @@
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9119,7 +9158,7 @@
         <xdr:cNvPr id="4" name="Диаграмма 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9157,7 +9196,7 @@
         <xdr:cNvPr id="6" name="Диаграмма 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9195,7 +9234,7 @@
         <xdr:cNvPr id="7" name="Диаграмма 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9233,7 +9272,7 @@
         <xdr:cNvPr id="5" name="Схема 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9269,7 +9308,7 @@
         <xdr:cNvPr id="8" name="Диаграмма 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9307,7 +9346,7 @@
         <xdr:cNvPr id="9" name="Диаграмма 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9345,7 +9384,7 @@
         <xdr:cNvPr id="10" name="Диаграмма 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9383,7 +9422,7 @@
         <xdr:cNvPr id="11" name="Диаграмма 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9421,7 +9460,7 @@
         <xdr:cNvPr id="12" name="Диаграмма 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9459,7 +9498,7 @@
         <xdr:cNvPr id="13" name="Диаграмма 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9497,7 +9536,7 @@
         <xdr:cNvPr id="14" name="Диаграмма 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9535,7 +9574,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC43166-386D-411A-B227-539522D3FB10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BC43166-386D-411A-B227-539522D3FB10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9585,7 +9624,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E95BF64-4F79-4800-AC1E-8E19A629802F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E95BF64-4F79-4800-AC1E-8E19A629802F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9635,7 +9674,7 @@
         <xdr:cNvPr id="16" name="Рисунок 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9103CE6E-4790-45E0-809E-B23A30CB78BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9103CE6E-4790-45E0-809E-B23A30CB78BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9685,7 +9724,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{043C28BA-C151-4B3A-846A-09440383AC7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{043C28BA-C151-4B3A-846A-09440383AC7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9735,7 +9774,7 @@
         <xdr:cNvPr id="18" name="Рисунок 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E30DD45-B474-45C7-8D79-CB3F1594DB7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8E30DD45-B474-45C7-8D79-CB3F1594DB7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9785,7 +9824,7 @@
         <xdr:cNvPr id="20" name="Рисунок 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99460B1B-52A8-4A8E-986E-09BE45BB37B3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{99460B1B-52A8-4A8E-986E-09BE45BB37B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9835,7 +9874,7 @@
         <xdr:cNvPr id="21" name="Рисунок 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20E30447-CD79-4006-A168-D73F027DFFB8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20E30447-CD79-4006-A168-D73F027DFFB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9885,7 +9924,7 @@
         <xdr:cNvPr id="22" name="Рисунок 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D3EE49-AE37-495B-986D-FA409FF446DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{76D3EE49-AE37-495B-986D-FA409FF446DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10220,8 +10259,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="B1:W399"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A229" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P283" sqref="P283"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10248,18 +10287,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="8:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="4:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="D31" s="39"/>
+      <c r="D31" s="38"/>
     </row>
     <row r="32" spans="4:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="D32" s="39"/>
+      <c r="D32" s="38"/>
     </row>
     <row r="36" spans="7:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G36" s="40" t="s">
+      <c r="G36" s="39" t="s">
         <v>73</v>
       </c>
     </row>
@@ -10267,12 +10306,12 @@
       <c r="D63" s="1"/>
     </row>
     <row r="70" spans="8:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H70" s="40" t="s">
+      <c r="H70" s="39" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="85" spans="8:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H85" s="40" t="s">
+      <c r="H85" s="39" t="s">
         <v>8</v>
       </c>
     </row>
@@ -10295,51 +10334,51 @@
     <row r="106" spans="7:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="107" spans="7:17" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="K110" s="125"/>
-      <c r="L110" s="125"/>
-      <c r="M110" s="125"/>
-      <c r="N110" s="125"/>
-      <c r="O110" s="125"/>
+      <c r="K110" s="95"/>
+      <c r="L110" s="95"/>
+      <c r="M110" s="95"/>
+      <c r="N110" s="95"/>
+      <c r="O110" s="95"/>
     </row>
     <row r="113" spans="9:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K113" s="125"/>
-      <c r="L113" s="125"/>
-      <c r="M113" s="125"/>
-      <c r="N113" s="125"/>
-      <c r="O113" s="125"/>
+      <c r="K113" s="95"/>
+      <c r="L113" s="95"/>
+      <c r="M113" s="95"/>
+      <c r="N113" s="95"/>
+      <c r="O113" s="95"/>
     </row>
     <row r="116" spans="9:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="K116" s="126"/>
-      <c r="L116" s="126"/>
-      <c r="M116" s="126"/>
-      <c r="N116" s="126"/>
-      <c r="O116" s="126"/>
+      <c r="K116" s="96"/>
+      <c r="L116" s="96"/>
+      <c r="M116" s="96"/>
+      <c r="N116" s="96"/>
+      <c r="O116" s="96"/>
     </row>
     <row r="120" spans="9:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="K120" s="125"/>
-      <c r="L120" s="125"/>
-      <c r="M120" s="125"/>
-      <c r="N120" s="125"/>
-      <c r="O120" s="125"/>
+      <c r="K120" s="95"/>
+      <c r="L120" s="95"/>
+      <c r="M120" s="95"/>
+      <c r="N120" s="95"/>
+      <c r="O120" s="95"/>
     </row>
     <row r="124" spans="9:15" ht="21" x14ac:dyDescent="0.35">
       <c r="I124" s="18"/>
       <c r="J124" s="18"/>
-      <c r="K124" s="124"/>
-      <c r="L124" s="124"/>
-      <c r="M124" s="124"/>
-      <c r="N124" s="124"/>
-      <c r="O124" s="124"/>
+      <c r="K124" s="94"/>
+      <c r="L124" s="94"/>
+      <c r="M124" s="94"/>
+      <c r="N124" s="94"/>
+      <c r="O124" s="94"/>
     </row>
     <row r="127" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="9:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="I128" s="116"/>
-      <c r="J128" s="116"/>
-      <c r="K128" s="116"/>
-      <c r="L128" s="116"/>
-      <c r="M128" s="116"/>
-      <c r="N128" s="116"/>
-      <c r="O128" s="116"/>
+      <c r="I128" s="99"/>
+      <c r="J128" s="99"/>
+      <c r="K128" s="99"/>
+      <c r="L128" s="99"/>
+      <c r="M128" s="99"/>
+      <c r="N128" s="99"/>
+      <c r="O128" s="99"/>
     </row>
     <row r="129" spans="6:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K129" s="15"/>
@@ -10350,32 +10389,32 @@
     <row r="134" spans="6:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="136" spans="6:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="137" spans="6:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F137" s="117" t="s">
+      <c r="F137" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="G137" s="117"/>
-      <c r="H137" s="117" t="s">
+      <c r="G137" s="100"/>
+      <c r="H137" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="I137" s="117"/>
-      <c r="J137" s="117"/>
-      <c r="K137" s="117"/>
-      <c r="L137" s="117" t="s">
+      <c r="I137" s="100"/>
+      <c r="J137" s="100"/>
+      <c r="K137" s="100"/>
+      <c r="L137" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="M137" s="117"/>
-      <c r="N137" s="44"/>
+      <c r="M137" s="100"/>
+      <c r="N137" s="41"/>
     </row>
     <row r="138" spans="6:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F138" s="118"/>
-      <c r="G138" s="118"/>
-      <c r="H138" s="118"/>
-      <c r="I138" s="118"/>
-      <c r="J138" s="118"/>
-      <c r="K138" s="118"/>
-      <c r="L138" s="118"/>
-      <c r="M138" s="118"/>
-      <c r="N138" s="45"/>
+      <c r="F138" s="93"/>
+      <c r="G138" s="93"/>
+      <c r="H138" s="93"/>
+      <c r="I138" s="93"/>
+      <c r="J138" s="93"/>
+      <c r="K138" s="93"/>
+      <c r="L138" s="93"/>
+      <c r="M138" s="93"/>
+      <c r="N138" s="42"/>
     </row>
     <row r="139" spans="6:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F139" s="16"/>
@@ -10384,7 +10423,7 @@
       <c r="I139" s="16"/>
       <c r="J139" s="17"/>
       <c r="K139" s="16"/>
-      <c r="L139" s="57"/>
+      <c r="L139" s="54"/>
       <c r="M139" s="16"/>
       <c r="N139" s="20"/>
     </row>
@@ -10395,117 +10434,117 @@
       <c r="I140" s="16"/>
       <c r="J140" s="17"/>
       <c r="K140" s="16"/>
-      <c r="L140" s="57"/>
+      <c r="L140" s="54"/>
       <c r="M140" s="16"/>
       <c r="N140" s="20"/>
     </row>
     <row r="141" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="N141" s="46"/>
+      <c r="N141" s="43"/>
     </row>
     <row r="142" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="N142" s="46"/>
+      <c r="N142" s="43"/>
     </row>
     <row r="143" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F143" s="127"/>
-      <c r="G143" s="127"/>
-      <c r="H143" s="118" t="s">
+      <c r="F143" s="81"/>
+      <c r="G143" s="81"/>
+      <c r="H143" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="I143" s="118"/>
-      <c r="J143" s="118"/>
-      <c r="K143" s="118"/>
-      <c r="L143" s="127"/>
-      <c r="M143" s="127"/>
-      <c r="N143" s="46"/>
+      <c r="I143" s="93"/>
+      <c r="J143" s="93"/>
+      <c r="K143" s="93"/>
+      <c r="L143" s="81"/>
+      <c r="M143" s="81"/>
+      <c r="N143" s="43"/>
     </row>
     <row r="144" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F144" s="119"/>
-      <c r="G144" s="119"/>
-      <c r="H144" s="128" t="s">
+      <c r="F144" s="82"/>
+      <c r="G144" s="82"/>
+      <c r="H144" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I144" s="128"/>
-      <c r="J144" s="128"/>
-      <c r="K144" s="128"/>
-      <c r="L144" s="119"/>
-      <c r="M144" s="119"/>
-      <c r="N144" s="46"/>
+      <c r="I144" s="92"/>
+      <c r="J144" s="92"/>
+      <c r="K144" s="92"/>
+      <c r="L144" s="82"/>
+      <c r="M144" s="82"/>
+      <c r="N144" s="43"/>
     </row>
     <row r="145" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F145" s="127"/>
-      <c r="G145" s="127"/>
-      <c r="H145" s="118" t="s">
+      <c r="F145" s="81"/>
+      <c r="G145" s="81"/>
+      <c r="H145" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="I145" s="118"/>
-      <c r="J145" s="118"/>
-      <c r="K145" s="118"/>
-      <c r="L145" s="127"/>
-      <c r="M145" s="127"/>
-      <c r="N145" s="46"/>
+      <c r="I145" s="93"/>
+      <c r="J145" s="93"/>
+      <c r="K145" s="93"/>
+      <c r="L145" s="81"/>
+      <c r="M145" s="81"/>
+      <c r="N145" s="43"/>
     </row>
     <row r="146" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F146" s="119"/>
-      <c r="G146" s="119"/>
-      <c r="H146" s="128" t="s">
+      <c r="F146" s="82"/>
+      <c r="G146" s="82"/>
+      <c r="H146" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="I146" s="128"/>
-      <c r="J146" s="128"/>
-      <c r="K146" s="128"/>
-      <c r="L146" s="119"/>
-      <c r="M146" s="119"/>
-      <c r="N146" s="46"/>
+      <c r="I146" s="92"/>
+      <c r="J146" s="92"/>
+      <c r="K146" s="92"/>
+      <c r="L146" s="82"/>
+      <c r="M146" s="82"/>
+      <c r="N146" s="43"/>
     </row>
     <row r="147" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F147" s="127"/>
-      <c r="G147" s="127"/>
-      <c r="H147" s="118" t="s">
+      <c r="F147" s="81"/>
+      <c r="G147" s="81"/>
+      <c r="H147" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="I147" s="118"/>
-      <c r="J147" s="118"/>
-      <c r="K147" s="118"/>
-      <c r="L147" s="127"/>
-      <c r="M147" s="127"/>
-      <c r="N147" s="46"/>
+      <c r="I147" s="93"/>
+      <c r="J147" s="93"/>
+      <c r="K147" s="93"/>
+      <c r="L147" s="81"/>
+      <c r="M147" s="81"/>
+      <c r="N147" s="43"/>
     </row>
     <row r="148" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F148" s="119"/>
-      <c r="G148" s="119"/>
-      <c r="H148" s="128" t="s">
+      <c r="F148" s="82"/>
+      <c r="G148" s="82"/>
+      <c r="H148" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="I148" s="128"/>
-      <c r="J148" s="128"/>
-      <c r="K148" s="128"/>
-      <c r="L148" s="119"/>
-      <c r="M148" s="119"/>
-      <c r="N148" s="46"/>
+      <c r="I148" s="92"/>
+      <c r="J148" s="92"/>
+      <c r="K148" s="92"/>
+      <c r="L148" s="82"/>
+      <c r="M148" s="82"/>
+      <c r="N148" s="43"/>
     </row>
     <row r="149" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F149" s="127"/>
-      <c r="G149" s="127"/>
-      <c r="H149" s="118" t="s">
+      <c r="F149" s="81"/>
+      <c r="G149" s="81"/>
+      <c r="H149" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="I149" s="118"/>
-      <c r="J149" s="118"/>
-      <c r="K149" s="118"/>
-      <c r="L149" s="127"/>
-      <c r="M149" s="127"/>
+      <c r="I149" s="93"/>
+      <c r="J149" s="93"/>
+      <c r="K149" s="93"/>
+      <c r="L149" s="81"/>
+      <c r="M149" s="81"/>
     </row>
     <row r="150" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F150" s="119"/>
-      <c r="G150" s="119"/>
-      <c r="H150" s="128" t="s">
+      <c r="F150" s="82"/>
+      <c r="G150" s="82"/>
+      <c r="H150" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="I150" s="128"/>
-      <c r="J150" s="128"/>
-      <c r="K150" s="128"/>
-      <c r="L150" s="119"/>
-      <c r="M150" s="119"/>
+      <c r="I150" s="92"/>
+      <c r="J150" s="92"/>
+      <c r="K150" s="92"/>
+      <c r="L150" s="82"/>
+      <c r="M150" s="82"/>
     </row>
     <row r="162" spans="5:23" ht="23.25" x14ac:dyDescent="0.25">
       <c r="H162" s="21" t="s">
@@ -10585,26 +10624,26 @@
       </c>
     </row>
     <row r="203" spans="2:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="D203" s="120" t="s">
+      <c r="D203" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="E203" s="120"/>
-      <c r="F203" s="120"/>
-      <c r="G203" s="121"/>
-      <c r="H203" s="122" t="s">
+      <c r="E203" s="85"/>
+      <c r="F203" s="85"/>
+      <c r="G203" s="102"/>
+      <c r="H203" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="I203" s="120"/>
-      <c r="J203" s="120"/>
-      <c r="K203" s="123"/>
-      <c r="L203" s="136" t="s">
+      <c r="I203" s="85"/>
+      <c r="J203" s="85"/>
+      <c r="K203" s="86"/>
+      <c r="L203" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="M203" s="120"/>
-      <c r="N203" s="120"/>
-      <c r="O203" s="120"/>
-      <c r="P203" s="120"/>
-      <c r="Q203" s="123"/>
+      <c r="M203" s="85"/>
+      <c r="N203" s="85"/>
+      <c r="O203" s="85"/>
+      <c r="P203" s="85"/>
+      <c r="Q203" s="86"/>
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E204" s="25"/>
@@ -10689,62 +10728,62 @@
       <c r="Q210" s="27"/>
     </row>
     <row r="211" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B211" s="47"/>
-      <c r="C211" s="47"/>
-      <c r="D211" s="50" t="s">
+      <c r="B211" s="44"/>
+      <c r="C211" s="44"/>
+      <c r="D211" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="E211" s="87"/>
-      <c r="F211" s="110"/>
-      <c r="G211" s="110"/>
-      <c r="H211" s="48"/>
-      <c r="I211" s="110"/>
-      <c r="J211" s="110"/>
-      <c r="K211" s="110"/>
-      <c r="L211" s="55"/>
-      <c r="M211" s="48"/>
-      <c r="N211" s="48"/>
-      <c r="O211" s="110"/>
-      <c r="P211" s="110"/>
-      <c r="Q211" s="110"/>
+      <c r="E211" s="59"/>
+      <c r="F211" s="101"/>
+      <c r="G211" s="101"/>
+      <c r="H211" s="45"/>
+      <c r="I211" s="101"/>
+      <c r="J211" s="101"/>
+      <c r="K211" s="101"/>
+      <c r="L211" s="52"/>
+      <c r="M211" s="45"/>
+      <c r="N211" s="45"/>
+      <c r="O211" s="101"/>
+      <c r="P211" s="101"/>
+      <c r="Q211" s="101"/>
     </row>
     <row r="212" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B212" s="47"/>
-      <c r="C212" s="47"/>
-      <c r="D212" s="51" t="s">
+      <c r="B212" s="44"/>
+      <c r="C212" s="44"/>
+      <c r="D212" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="E212" s="88"/>
-      <c r="F212" s="109"/>
-      <c r="G212" s="109"/>
-      <c r="H212" s="49"/>
-      <c r="I212" s="109"/>
-      <c r="J212" s="109"/>
-      <c r="K212" s="109"/>
-      <c r="L212" s="56"/>
-      <c r="M212" s="49"/>
-      <c r="N212" s="49"/>
-      <c r="O212" s="109"/>
-      <c r="P212" s="109"/>
-      <c r="Q212" s="109"/>
+      <c r="E212" s="60"/>
+      <c r="F212" s="104"/>
+      <c r="G212" s="104"/>
+      <c r="H212" s="46"/>
+      <c r="I212" s="104"/>
+      <c r="J212" s="104"/>
+      <c r="K212" s="104"/>
+      <c r="L212" s="53"/>
+      <c r="M212" s="46"/>
+      <c r="N212" s="46"/>
+      <c r="O212" s="104"/>
+      <c r="P212" s="104"/>
+      <c r="Q212" s="104"/>
     </row>
     <row r="213" spans="2:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D213" s="50" t="s">
+      <c r="D213" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="E213" s="87"/>
-      <c r="F213" s="110"/>
-      <c r="G213" s="110"/>
-      <c r="H213" s="48"/>
-      <c r="I213" s="110"/>
-      <c r="J213" s="110"/>
-      <c r="K213" s="110"/>
-      <c r="L213" s="55"/>
-      <c r="M213" s="48"/>
-      <c r="N213" s="48"/>
-      <c r="O213" s="110"/>
-      <c r="P213" s="110"/>
-      <c r="Q213" s="110"/>
+      <c r="E213" s="59"/>
+      <c r="F213" s="101"/>
+      <c r="G213" s="101"/>
+      <c r="H213" s="45"/>
+      <c r="I213" s="101"/>
+      <c r="J213" s="101"/>
+      <c r="K213" s="101"/>
+      <c r="L213" s="52"/>
+      <c r="M213" s="45"/>
+      <c r="N213" s="45"/>
+      <c r="O213" s="101"/>
+      <c r="P213" s="101"/>
+      <c r="Q213" s="101"/>
     </row>
     <row r="215" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
@@ -10764,28 +10803,28 @@
       <c r="N229" s="23"/>
     </row>
     <row r="252" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D252" s="54" t="s">
+      <c r="D252" s="51" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="253" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D253" s="54" t="s">
+      <c r="D253" s="51" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="259" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E259" s="53"/>
-      <c r="F259" s="53"/>
-      <c r="G259" s="53"/>
-      <c r="I259" s="54"/>
-      <c r="J259" s="52"/>
+      <c r="E259" s="50"/>
+      <c r="F259" s="50"/>
+      <c r="G259" s="50"/>
+      <c r="I259" s="51"/>
+      <c r="J259" s="49"/>
     </row>
     <row r="260" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E260" s="53"/>
-      <c r="F260" s="53"/>
-      <c r="G260" s="53"/>
-      <c r="I260" s="54"/>
-      <c r="J260" s="52"/>
+      <c r="E260" s="50"/>
+      <c r="F260" s="50"/>
+      <c r="G260" s="50"/>
+      <c r="I260" s="51"/>
+      <c r="J260" s="49"/>
     </row>
     <row r="263" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H263" s="21" t="s">
@@ -10799,17 +10838,17 @@
       <c r="N263" s="23"/>
     </row>
     <row r="266" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B266" s="131" t="s">
+      <c r="B266" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="C266" s="131"/>
-      <c r="D266" s="131"/>
-      <c r="E266" s="39"/>
-      <c r="F266" s="39"/>
-      <c r="G266" s="131" t="s">
+      <c r="C266" s="89"/>
+      <c r="D266" s="89"/>
+      <c r="E266" s="38"/>
+      <c r="F266" s="38"/>
+      <c r="G266" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="H266" s="131"/>
+      <c r="H266" s="89"/>
     </row>
     <row r="267" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E267" s="35"/>
@@ -10848,23 +10887,23 @@
       <c r="E278" s="35"/>
     </row>
     <row r="279" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B279" s="133" t="s">
+      <c r="B279" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="C279" s="133"/>
-      <c r="D279" s="133"/>
+      <c r="C279" s="91"/>
+      <c r="D279" s="91"/>
       <c r="E279" s="35"/>
-      <c r="G279" s="133" t="s">
+      <c r="G279" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="H279" s="133"/>
+      <c r="H279" s="91"/>
     </row>
     <row r="280" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B280" s="132"/>
-      <c r="C280" s="132"/>
-      <c r="D280" s="132"/>
-      <c r="G280" s="132"/>
-      <c r="H280" s="132"/>
+      <c r="B280" s="90"/>
+      <c r="C280" s="90"/>
+      <c r="D280" s="90"/>
+      <c r="G280" s="90"/>
+      <c r="H280" s="90"/>
     </row>
     <row r="282" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C282" s="24"/>
@@ -10883,16 +10922,16 @@
       <c r="B285" s="24"/>
     </row>
     <row r="291" spans="8:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H291" s="58" t="s">
+      <c r="H291" s="55" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="297" spans="8:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="I297" s="58"/>
-      <c r="J297" s="58"/>
-      <c r="K297" s="58"/>
-      <c r="L297" s="58"/>
-      <c r="M297" s="58"/>
+      <c r="I297" s="55"/>
+      <c r="J297" s="55"/>
+      <c r="K297" s="55"/>
+      <c r="L297" s="55"/>
+      <c r="M297" s="55"/>
     </row>
     <row r="317" spans="4:4" ht="21" x14ac:dyDescent="0.35">
       <c r="D317" s="22"/>
@@ -10901,7 +10940,7 @@
       <c r="D318" s="22"/>
     </row>
     <row r="325" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H325" s="58" t="s">
+      <c r="H325" s="55" t="s">
         <v>50</v>
       </c>
     </row>
@@ -10939,498 +10978,515 @@
       </c>
     </row>
     <row r="358" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H358" s="58" t="s">
+      <c r="H358" s="55" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="360" spans="2:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B360" s="112" t="s">
+      <c r="B360" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="C360" s="112"/>
-      <c r="D360" s="112"/>
-      <c r="E360" s="112"/>
-      <c r="F360" s="112"/>
-      <c r="G360" s="112"/>
-      <c r="H360" s="114"/>
-      <c r="I360" s="114"/>
+      <c r="C360" s="83"/>
+      <c r="D360" s="83"/>
+      <c r="E360" s="83"/>
+      <c r="F360" s="83"/>
+      <c r="G360" s="83"/>
+      <c r="H360" s="107"/>
+      <c r="I360" s="107"/>
     </row>
     <row r="361" spans="2:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B361" s="129" t="s">
+      <c r="B361" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C361" s="129"/>
-      <c r="D361" s="129"/>
-      <c r="E361" s="129"/>
-      <c r="F361" s="129"/>
-      <c r="G361" s="129"/>
-      <c r="H361" s="115"/>
-      <c r="I361" s="115"/>
-      <c r="K361" s="54"/>
-      <c r="L361" s="54"/>
-      <c r="M361" s="54"/>
-      <c r="N361" s="54"/>
-      <c r="O361" s="54"/>
+      <c r="C361" s="87"/>
+      <c r="D361" s="87"/>
+      <c r="E361" s="87"/>
+      <c r="F361" s="87"/>
+      <c r="G361" s="87"/>
+      <c r="H361" s="108"/>
+      <c r="I361" s="108"/>
+      <c r="K361" s="51"/>
+      <c r="L361" s="51"/>
+      <c r="M361" s="51"/>
+      <c r="N361" s="51"/>
+      <c r="O361" s="51"/>
     </row>
     <row r="362" spans="2:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B362" s="130" t="s">
+      <c r="B362" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="C362" s="130"/>
-      <c r="D362" s="130"/>
-      <c r="E362" s="130"/>
-      <c r="F362" s="130"/>
-      <c r="G362" s="130"/>
-      <c r="H362" s="114"/>
-      <c r="I362" s="114"/>
+      <c r="C362" s="88"/>
+      <c r="D362" s="88"/>
+      <c r="E362" s="88"/>
+      <c r="F362" s="88"/>
+      <c r="G362" s="88"/>
+      <c r="H362" s="107"/>
+      <c r="I362" s="107"/>
     </row>
     <row r="364" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="365" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="366" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="368" spans="2:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K368" s="112" t="s">
+      <c r="K368" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="L368" s="112"/>
-      <c r="M368" s="112"/>
-      <c r="N368" s="112"/>
-      <c r="O368" s="112"/>
-      <c r="P368" s="113"/>
-      <c r="Q368" s="113"/>
-      <c r="R368" s="113"/>
+      <c r="L368" s="83"/>
+      <c r="M368" s="83"/>
+      <c r="N368" s="83"/>
+      <c r="O368" s="83"/>
+      <c r="P368" s="106"/>
+      <c r="Q368" s="106"/>
+      <c r="R368" s="106"/>
     </row>
     <row r="369" spans="2:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K369" s="111" t="s">
+      <c r="K369" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="L369" s="111"/>
-      <c r="M369" s="111"/>
-      <c r="N369" s="111"/>
-      <c r="O369" s="111"/>
-      <c r="P369" s="134"/>
-      <c r="Q369" s="134"/>
-      <c r="R369" s="134"/>
+      <c r="L369" s="105"/>
+      <c r="M369" s="105"/>
+      <c r="N369" s="105"/>
+      <c r="O369" s="105"/>
+      <c r="P369" s="79"/>
+      <c r="Q369" s="79"/>
+      <c r="R369" s="79"/>
     </row>
     <row r="370" spans="2:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K370" s="112" t="s">
+      <c r="K370" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="L370" s="112"/>
-      <c r="M370" s="112"/>
-      <c r="N370" s="112"/>
-      <c r="O370" s="112"/>
-      <c r="P370" s="135"/>
-      <c r="Q370" s="135"/>
-      <c r="R370" s="135"/>
+      <c r="L370" s="83"/>
+      <c r="M370" s="83"/>
+      <c r="N370" s="83"/>
+      <c r="O370" s="83"/>
+      <c r="P370" s="80"/>
+      <c r="Q370" s="80"/>
+      <c r="R370" s="80"/>
     </row>
     <row r="380" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="H380" s="58" t="s">
+      <c r="H380" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="I380" s="58"/>
-      <c r="J380" s="58"/>
-      <c r="K380" s="58"/>
-      <c r="L380" s="58"/>
-      <c r="M380" s="58"/>
+      <c r="I380" s="55"/>
+      <c r="J380" s="55"/>
+      <c r="K380" s="55"/>
+      <c r="L380" s="55"/>
+      <c r="M380" s="55"/>
       <c r="N380" s="37"/>
     </row>
     <row r="383" spans="2:20" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B383" s="107" t="s">
+      <c r="B383" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="C383" s="107"/>
-      <c r="D383" s="107"/>
-      <c r="E383" s="107"/>
-      <c r="F383" s="107" t="s">
+      <c r="C383" s="98"/>
+      <c r="D383" s="98"/>
+      <c r="E383" s="98"/>
+      <c r="F383" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="G383" s="107"/>
-      <c r="H383" s="107"/>
-      <c r="I383" s="107" t="s">
+      <c r="G383" s="98"/>
+      <c r="H383" s="98"/>
+      <c r="I383" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="J383" s="107"/>
-      <c r="K383" s="68" t="s">
+      <c r="J383" s="98"/>
+      <c r="K383" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="L383" s="108" t="s">
+      <c r="L383" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="M383" s="108"/>
-      <c r="N383" s="108" t="s">
+      <c r="M383" s="97"/>
+      <c r="N383" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="O383" s="108"/>
-      <c r="P383" s="107" t="s">
+      <c r="O383" s="97"/>
+      <c r="P383" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="Q383" s="107"/>
-      <c r="R383" s="69" t="s">
+      <c r="Q383" s="98"/>
+      <c r="R383" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="S383" s="108" t="s">
+      <c r="S383" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="T383" s="108"/>
+      <c r="T383" s="97"/>
     </row>
     <row r="384" spans="2:20" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B384" s="67"/>
-      <c r="C384" s="67"/>
-      <c r="D384" s="67"/>
-      <c r="E384" s="67"/>
-      <c r="F384" s="67"/>
-      <c r="G384" s="67"/>
-      <c r="H384" s="67"/>
-      <c r="I384" s="67"/>
-      <c r="J384" s="67"/>
-      <c r="K384" s="67"/>
-      <c r="L384" s="67"/>
-      <c r="M384" s="67"/>
-      <c r="N384" s="67"/>
-      <c r="O384" s="67"/>
-      <c r="P384" s="67"/>
-      <c r="Q384" s="67"/>
-      <c r="R384" s="67"/>
-      <c r="S384" s="67"/>
-      <c r="T384" s="67"/>
+      <c r="B384" s="56"/>
+      <c r="C384" s="56"/>
+      <c r="D384" s="56"/>
+      <c r="E384" s="56"/>
+      <c r="F384" s="56"/>
+      <c r="G384" s="56"/>
+      <c r="H384" s="56"/>
+      <c r="I384" s="56"/>
+      <c r="J384" s="56"/>
+      <c r="K384" s="56"/>
+      <c r="L384" s="56"/>
+      <c r="M384" s="56"/>
+      <c r="N384" s="56"/>
+      <c r="O384" s="56"/>
+      <c r="P384" s="56"/>
+      <c r="Q384" s="56"/>
+      <c r="R384" s="56"/>
+      <c r="S384" s="56"/>
+      <c r="T384" s="56"/>
     </row>
     <row r="385" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B385" s="67"/>
-      <c r="C385" s="67"/>
-      <c r="D385" s="67"/>
-      <c r="E385" s="67"/>
-      <c r="F385" s="67"/>
-      <c r="G385" s="67"/>
-      <c r="H385" s="67"/>
-      <c r="I385" s="67"/>
-      <c r="J385" s="67"/>
-      <c r="K385" s="67"/>
-      <c r="L385" s="67"/>
-      <c r="M385" s="67"/>
-      <c r="N385" s="67"/>
-      <c r="O385" s="67"/>
-      <c r="P385" s="67"/>
-      <c r="Q385" s="67"/>
-      <c r="R385" s="67"/>
-      <c r="S385" s="67"/>
-      <c r="T385" s="67"/>
+      <c r="B385" s="56"/>
+      <c r="C385" s="56"/>
+      <c r="D385" s="56"/>
+      <c r="E385" s="56"/>
+      <c r="F385" s="56"/>
+      <c r="G385" s="56"/>
+      <c r="H385" s="56"/>
+      <c r="I385" s="56"/>
+      <c r="J385" s="56"/>
+      <c r="K385" s="56"/>
+      <c r="L385" s="56"/>
+      <c r="M385" s="56"/>
+      <c r="N385" s="56"/>
+      <c r="O385" s="56"/>
+      <c r="P385" s="56"/>
+      <c r="Q385" s="56"/>
+      <c r="R385" s="56"/>
+      <c r="S385" s="56"/>
+      <c r="T385" s="56"/>
     </row>
     <row r="386" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B386" s="67"/>
-      <c r="C386" s="67"/>
-      <c r="D386" s="67"/>
-      <c r="E386" s="67"/>
-      <c r="F386" s="67"/>
-      <c r="G386" s="67"/>
-      <c r="H386" s="67"/>
-      <c r="I386" s="67"/>
-      <c r="J386" s="67"/>
-      <c r="K386" s="67"/>
-      <c r="L386" s="67"/>
-      <c r="M386" s="67"/>
-      <c r="N386" s="67"/>
-      <c r="O386" s="67"/>
-      <c r="P386" s="67"/>
-      <c r="Q386" s="67"/>
-      <c r="R386" s="67"/>
-      <c r="S386" s="67"/>
-      <c r="T386" s="67"/>
+      <c r="B386" s="56"/>
+      <c r="C386" s="56"/>
+      <c r="D386" s="56"/>
+      <c r="E386" s="56"/>
+      <c r="F386" s="56"/>
+      <c r="G386" s="56"/>
+      <c r="H386" s="56"/>
+      <c r="I386" s="56"/>
+      <c r="J386" s="56"/>
+      <c r="K386" s="56"/>
+      <c r="L386" s="56"/>
+      <c r="M386" s="56"/>
+      <c r="N386" s="56"/>
+      <c r="O386" s="56"/>
+      <c r="P386" s="56"/>
+      <c r="Q386" s="56"/>
+      <c r="R386" s="56"/>
+      <c r="S386" s="56"/>
+      <c r="T386" s="56"/>
     </row>
     <row r="387" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B387" s="67"/>
-      <c r="C387" s="67"/>
-      <c r="D387" s="67"/>
-      <c r="E387" s="67"/>
-      <c r="F387" s="67"/>
-      <c r="G387" s="67"/>
-      <c r="H387" s="67"/>
-      <c r="I387" s="67"/>
-      <c r="J387" s="67"/>
-      <c r="K387" s="67"/>
-      <c r="L387" s="67"/>
-      <c r="M387" s="67"/>
-      <c r="N387" s="67"/>
-      <c r="O387" s="67"/>
-      <c r="P387" s="67"/>
-      <c r="Q387" s="67"/>
-      <c r="R387" s="67"/>
-      <c r="S387" s="67"/>
-      <c r="T387" s="67"/>
+      <c r="B387" s="56"/>
+      <c r="C387" s="56"/>
+      <c r="D387" s="56"/>
+      <c r="E387" s="56"/>
+      <c r="F387" s="56"/>
+      <c r="G387" s="56"/>
+      <c r="H387" s="56"/>
+      <c r="I387" s="56"/>
+      <c r="J387" s="56"/>
+      <c r="K387" s="56"/>
+      <c r="L387" s="56"/>
+      <c r="M387" s="56"/>
+      <c r="N387" s="56"/>
+      <c r="O387" s="56"/>
+      <c r="P387" s="56"/>
+      <c r="Q387" s="56"/>
+      <c r="R387" s="56"/>
+      <c r="S387" s="56"/>
+      <c r="T387" s="56"/>
     </row>
     <row r="388" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B388" s="67"/>
-      <c r="C388" s="67"/>
-      <c r="D388" s="67"/>
-      <c r="E388" s="67"/>
-      <c r="F388" s="67"/>
-      <c r="G388" s="67"/>
-      <c r="H388" s="67"/>
-      <c r="I388" s="67"/>
-      <c r="J388" s="67"/>
-      <c r="K388" s="67"/>
-      <c r="L388" s="67"/>
-      <c r="M388" s="67"/>
-      <c r="N388" s="67"/>
-      <c r="O388" s="67"/>
-      <c r="P388" s="67"/>
-      <c r="Q388" s="67"/>
-      <c r="R388" s="67"/>
-      <c r="S388" s="67"/>
-      <c r="T388" s="67"/>
+      <c r="B388" s="56"/>
+      <c r="C388" s="56"/>
+      <c r="D388" s="56"/>
+      <c r="E388" s="56"/>
+      <c r="F388" s="56"/>
+      <c r="G388" s="56"/>
+      <c r="H388" s="56"/>
+      <c r="I388" s="56"/>
+      <c r="J388" s="56"/>
+      <c r="K388" s="56"/>
+      <c r="L388" s="56"/>
+      <c r="M388" s="56"/>
+      <c r="N388" s="56"/>
+      <c r="O388" s="56"/>
+      <c r="P388" s="56"/>
+      <c r="Q388" s="56"/>
+      <c r="R388" s="56"/>
+      <c r="S388" s="56"/>
+      <c r="T388" s="56"/>
     </row>
     <row r="389" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B389" s="67"/>
-      <c r="C389" s="67"/>
-      <c r="D389" s="67"/>
-      <c r="E389" s="67"/>
-      <c r="F389" s="67"/>
-      <c r="G389" s="67"/>
-      <c r="H389" s="67"/>
-      <c r="I389" s="67"/>
-      <c r="J389" s="67"/>
-      <c r="K389" s="67"/>
-      <c r="L389" s="67"/>
-      <c r="M389" s="67"/>
-      <c r="N389" s="67"/>
-      <c r="O389" s="67"/>
-      <c r="P389" s="67"/>
-      <c r="Q389" s="67"/>
-      <c r="R389" s="67"/>
-      <c r="S389" s="67"/>
-      <c r="T389" s="67"/>
+      <c r="B389" s="56"/>
+      <c r="C389" s="56"/>
+      <c r="D389" s="56"/>
+      <c r="E389" s="56"/>
+      <c r="F389" s="56"/>
+      <c r="G389" s="56"/>
+      <c r="H389" s="56"/>
+      <c r="I389" s="56"/>
+      <c r="J389" s="56"/>
+      <c r="K389" s="56"/>
+      <c r="L389" s="56"/>
+      <c r="M389" s="56"/>
+      <c r="N389" s="56"/>
+      <c r="O389" s="56"/>
+      <c r="P389" s="56"/>
+      <c r="Q389" s="56"/>
+      <c r="R389" s="56"/>
+      <c r="S389" s="56"/>
+      <c r="T389" s="56"/>
     </row>
     <row r="390" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B390" s="67"/>
-      <c r="C390" s="67"/>
-      <c r="D390" s="67"/>
-      <c r="E390" s="67"/>
-      <c r="F390" s="67"/>
-      <c r="G390" s="67"/>
-      <c r="H390" s="67"/>
-      <c r="I390" s="67"/>
-      <c r="J390" s="67"/>
-      <c r="K390" s="67"/>
-      <c r="L390" s="67"/>
-      <c r="M390" s="67"/>
-      <c r="N390" s="67"/>
-      <c r="O390" s="67"/>
-      <c r="P390" s="67"/>
-      <c r="Q390" s="67"/>
-      <c r="R390" s="67"/>
-      <c r="S390" s="67"/>
-      <c r="T390" s="67"/>
+      <c r="B390" s="56"/>
+      <c r="C390" s="56"/>
+      <c r="D390" s="56"/>
+      <c r="E390" s="56"/>
+      <c r="F390" s="56"/>
+      <c r="G390" s="56"/>
+      <c r="H390" s="56"/>
+      <c r="I390" s="56"/>
+      <c r="J390" s="56"/>
+      <c r="K390" s="56"/>
+      <c r="L390" s="56"/>
+      <c r="M390" s="56"/>
+      <c r="N390" s="56"/>
+      <c r="O390" s="56"/>
+      <c r="P390" s="56"/>
+      <c r="Q390" s="56"/>
+      <c r="R390" s="56"/>
+      <c r="S390" s="56"/>
+      <c r="T390" s="56"/>
     </row>
     <row r="391" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B391" s="67"/>
-      <c r="C391" s="67"/>
-      <c r="D391" s="67"/>
-      <c r="E391" s="67"/>
-      <c r="F391" s="67"/>
-      <c r="G391" s="67"/>
-      <c r="H391" s="67"/>
-      <c r="I391" s="67"/>
-      <c r="J391" s="67"/>
-      <c r="K391" s="67"/>
-      <c r="L391" s="67"/>
-      <c r="M391" s="67"/>
-      <c r="N391" s="67"/>
-      <c r="O391" s="67"/>
-      <c r="P391" s="67"/>
-      <c r="Q391" s="67"/>
-      <c r="R391" s="67"/>
-      <c r="S391" s="67"/>
-      <c r="T391" s="67"/>
+      <c r="B391" s="56"/>
+      <c r="C391" s="56"/>
+      <c r="D391" s="56"/>
+      <c r="E391" s="56"/>
+      <c r="F391" s="56"/>
+      <c r="G391" s="56"/>
+      <c r="H391" s="56"/>
+      <c r="I391" s="56"/>
+      <c r="J391" s="56"/>
+      <c r="K391" s="56"/>
+      <c r="L391" s="56"/>
+      <c r="M391" s="56"/>
+      <c r="N391" s="56"/>
+      <c r="O391" s="56"/>
+      <c r="P391" s="56"/>
+      <c r="Q391" s="56"/>
+      <c r="R391" s="56"/>
+      <c r="S391" s="56"/>
+      <c r="T391" s="56"/>
     </row>
     <row r="392" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B392" s="67"/>
-      <c r="C392" s="67"/>
-      <c r="D392" s="67"/>
-      <c r="E392" s="67"/>
-      <c r="F392" s="67"/>
-      <c r="G392" s="67"/>
-      <c r="H392" s="67"/>
-      <c r="I392" s="67"/>
-      <c r="J392" s="67"/>
-      <c r="K392" s="67"/>
-      <c r="L392" s="67"/>
-      <c r="M392" s="67"/>
-      <c r="N392" s="67"/>
-      <c r="O392" s="67"/>
-      <c r="P392" s="67"/>
-      <c r="Q392" s="67"/>
-      <c r="R392" s="67"/>
-      <c r="S392" s="67"/>
-      <c r="T392" s="67"/>
+      <c r="B392" s="56"/>
+      <c r="C392" s="56"/>
+      <c r="D392" s="56"/>
+      <c r="E392" s="56"/>
+      <c r="F392" s="56"/>
+      <c r="G392" s="56"/>
+      <c r="H392" s="56"/>
+      <c r="I392" s="56"/>
+      <c r="J392" s="56"/>
+      <c r="K392" s="56"/>
+      <c r="L392" s="56"/>
+      <c r="M392" s="56"/>
+      <c r="N392" s="56"/>
+      <c r="O392" s="56"/>
+      <c r="P392" s="56"/>
+      <c r="Q392" s="56"/>
+      <c r="R392" s="56"/>
+      <c r="S392" s="56"/>
+      <c r="T392" s="56"/>
     </row>
     <row r="393" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B393" s="67"/>
-      <c r="C393" s="67"/>
-      <c r="D393" s="67"/>
-      <c r="E393" s="67"/>
-      <c r="F393" s="67"/>
-      <c r="G393" s="67"/>
-      <c r="H393" s="67"/>
-      <c r="I393" s="67"/>
-      <c r="J393" s="67"/>
-      <c r="K393" s="67"/>
-      <c r="L393" s="67"/>
-      <c r="M393" s="67"/>
-      <c r="N393" s="67"/>
-      <c r="O393" s="67"/>
-      <c r="P393" s="67"/>
-      <c r="Q393" s="67"/>
-      <c r="R393" s="67"/>
-      <c r="S393" s="67"/>
-      <c r="T393" s="67"/>
+      <c r="B393" s="56"/>
+      <c r="C393" s="56"/>
+      <c r="D393" s="56"/>
+      <c r="E393" s="56"/>
+      <c r="F393" s="56"/>
+      <c r="G393" s="56"/>
+      <c r="H393" s="56"/>
+      <c r="I393" s="56"/>
+      <c r="J393" s="56"/>
+      <c r="K393" s="56"/>
+      <c r="L393" s="56"/>
+      <c r="M393" s="56"/>
+      <c r="N393" s="56"/>
+      <c r="O393" s="56"/>
+      <c r="P393" s="56"/>
+      <c r="Q393" s="56"/>
+      <c r="R393" s="56"/>
+      <c r="S393" s="56"/>
+      <c r="T393" s="56"/>
     </row>
     <row r="394" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B394" s="67"/>
-      <c r="C394" s="67"/>
-      <c r="D394" s="67"/>
-      <c r="E394" s="67"/>
-      <c r="F394" s="67"/>
-      <c r="G394" s="67"/>
-      <c r="H394" s="67"/>
-      <c r="I394" s="67"/>
-      <c r="J394" s="67"/>
-      <c r="K394" s="67"/>
-      <c r="L394" s="67"/>
-      <c r="M394" s="67"/>
-      <c r="N394" s="67"/>
-      <c r="O394" s="67"/>
-      <c r="P394" s="67"/>
-      <c r="Q394" s="67"/>
-      <c r="R394" s="67"/>
-      <c r="S394" s="67"/>
-      <c r="T394" s="67"/>
+      <c r="B394" s="56"/>
+      <c r="C394" s="56"/>
+      <c r="D394" s="56"/>
+      <c r="E394" s="56"/>
+      <c r="F394" s="56"/>
+      <c r="G394" s="56"/>
+      <c r="H394" s="56"/>
+      <c r="I394" s="56"/>
+      <c r="J394" s="56"/>
+      <c r="K394" s="56"/>
+      <c r="L394" s="56"/>
+      <c r="M394" s="56"/>
+      <c r="N394" s="56"/>
+      <c r="O394" s="56"/>
+      <c r="P394" s="56"/>
+      <c r="Q394" s="56"/>
+      <c r="R394" s="56"/>
+      <c r="S394" s="56"/>
+      <c r="T394" s="56"/>
     </row>
     <row r="395" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B395" s="67"/>
-      <c r="C395" s="67"/>
-      <c r="D395" s="67"/>
-      <c r="E395" s="67"/>
-      <c r="F395" s="67"/>
-      <c r="G395" s="67"/>
-      <c r="H395" s="67"/>
-      <c r="I395" s="67"/>
-      <c r="J395" s="67"/>
-      <c r="K395" s="67"/>
-      <c r="L395" s="67"/>
-      <c r="M395" s="67"/>
-      <c r="N395" s="67"/>
-      <c r="O395" s="67"/>
-      <c r="P395" s="67"/>
-      <c r="Q395" s="67"/>
-      <c r="R395" s="67"/>
-      <c r="S395" s="67"/>
-      <c r="T395" s="67"/>
+      <c r="B395" s="56"/>
+      <c r="C395" s="56"/>
+      <c r="D395" s="56"/>
+      <c r="E395" s="56"/>
+      <c r="F395" s="56"/>
+      <c r="G395" s="56"/>
+      <c r="H395" s="56"/>
+      <c r="I395" s="56"/>
+      <c r="J395" s="56"/>
+      <c r="K395" s="56"/>
+      <c r="L395" s="56"/>
+      <c r="M395" s="56"/>
+      <c r="N395" s="56"/>
+      <c r="O395" s="56"/>
+      <c r="P395" s="56"/>
+      <c r="Q395" s="56"/>
+      <c r="R395" s="56"/>
+      <c r="S395" s="56"/>
+      <c r="T395" s="56"/>
     </row>
     <row r="396" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B396" s="67"/>
-      <c r="C396" s="67"/>
-      <c r="D396" s="67"/>
-      <c r="E396" s="67"/>
-      <c r="F396" s="67"/>
-      <c r="G396" s="67"/>
-      <c r="H396" s="67"/>
-      <c r="I396" s="67"/>
-      <c r="J396" s="67"/>
-      <c r="K396" s="67"/>
-      <c r="L396" s="67"/>
-      <c r="M396" s="67"/>
-      <c r="N396" s="67"/>
-      <c r="O396" s="67"/>
-      <c r="P396" s="67"/>
-      <c r="Q396" s="67"/>
-      <c r="R396" s="67"/>
-      <c r="S396" s="67"/>
-      <c r="T396" s="67"/>
+      <c r="B396" s="56"/>
+      <c r="C396" s="56"/>
+      <c r="D396" s="56"/>
+      <c r="E396" s="56"/>
+      <c r="F396" s="56"/>
+      <c r="G396" s="56"/>
+      <c r="H396" s="56"/>
+      <c r="I396" s="56"/>
+      <c r="J396" s="56"/>
+      <c r="K396" s="56"/>
+      <c r="L396" s="56"/>
+      <c r="M396" s="56"/>
+      <c r="N396" s="56"/>
+      <c r="O396" s="56"/>
+      <c r="P396" s="56"/>
+      <c r="Q396" s="56"/>
+      <c r="R396" s="56"/>
+      <c r="S396" s="56"/>
+      <c r="T396" s="56"/>
     </row>
     <row r="397" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B397" s="67"/>
-      <c r="C397" s="67"/>
-      <c r="D397" s="67"/>
-      <c r="E397" s="67"/>
-      <c r="F397" s="67"/>
-      <c r="G397" s="67"/>
-      <c r="H397" s="67"/>
-      <c r="I397" s="67"/>
-      <c r="J397" s="67"/>
-      <c r="K397" s="67"/>
-      <c r="L397" s="67"/>
-      <c r="M397" s="67"/>
-      <c r="N397" s="67"/>
-      <c r="O397" s="67"/>
-      <c r="P397" s="67"/>
-      <c r="Q397" s="67"/>
-      <c r="R397" s="67"/>
-      <c r="S397" s="67"/>
-      <c r="T397" s="67"/>
+      <c r="B397" s="56"/>
+      <c r="C397" s="56"/>
+      <c r="D397" s="56"/>
+      <c r="E397" s="56"/>
+      <c r="F397" s="56"/>
+      <c r="G397" s="56"/>
+      <c r="H397" s="56"/>
+      <c r="I397" s="56"/>
+      <c r="J397" s="56"/>
+      <c r="K397" s="56"/>
+      <c r="L397" s="56"/>
+      <c r="M397" s="56"/>
+      <c r="N397" s="56"/>
+      <c r="O397" s="56"/>
+      <c r="P397" s="56"/>
+      <c r="Q397" s="56"/>
+      <c r="R397" s="56"/>
+      <c r="S397" s="56"/>
+      <c r="T397" s="56"/>
     </row>
     <row r="398" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B398" s="67"/>
-      <c r="C398" s="67"/>
-      <c r="D398" s="67"/>
-      <c r="E398" s="67"/>
-      <c r="F398" s="67"/>
-      <c r="G398" s="67"/>
-      <c r="H398" s="67"/>
-      <c r="I398" s="67"/>
-      <c r="J398" s="67"/>
-      <c r="K398" s="67"/>
-      <c r="L398" s="67"/>
-      <c r="M398" s="67"/>
-      <c r="N398" s="67"/>
-      <c r="O398" s="67"/>
-      <c r="P398" s="67"/>
-      <c r="Q398" s="67"/>
-      <c r="R398" s="67"/>
-      <c r="S398" s="67"/>
-      <c r="T398" s="67"/>
+      <c r="B398" s="56"/>
+      <c r="C398" s="56"/>
+      <c r="D398" s="56"/>
+      <c r="E398" s="56"/>
+      <c r="F398" s="56"/>
+      <c r="G398" s="56"/>
+      <c r="H398" s="56"/>
+      <c r="I398" s="56"/>
+      <c r="J398" s="56"/>
+      <c r="K398" s="56"/>
+      <c r="L398" s="56"/>
+      <c r="M398" s="56"/>
+      <c r="N398" s="56"/>
+      <c r="O398" s="56"/>
+      <c r="P398" s="56"/>
+      <c r="Q398" s="56"/>
+      <c r="R398" s="56"/>
+      <c r="S398" s="56"/>
+      <c r="T398" s="56"/>
     </row>
     <row r="399" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B399" s="67"/>
-      <c r="C399" s="67"/>
-      <c r="D399" s="67"/>
-      <c r="E399" s="67"/>
-      <c r="F399" s="67"/>
-      <c r="G399" s="67"/>
-      <c r="H399" s="67"/>
-      <c r="I399" s="67"/>
-      <c r="J399" s="67"/>
-      <c r="K399" s="67"/>
-      <c r="L399" s="67"/>
-      <c r="M399" s="67"/>
-      <c r="N399" s="67"/>
-      <c r="O399" s="67"/>
-      <c r="P399" s="67"/>
-      <c r="Q399" s="67"/>
-      <c r="R399" s="67"/>
-      <c r="S399" s="67"/>
-      <c r="T399" s="67"/>
+      <c r="B399" s="56"/>
+      <c r="C399" s="56"/>
+      <c r="D399" s="56"/>
+      <c r="E399" s="56"/>
+      <c r="F399" s="56"/>
+      <c r="G399" s="56"/>
+      <c r="H399" s="56"/>
+      <c r="I399" s="56"/>
+      <c r="J399" s="56"/>
+      <c r="K399" s="56"/>
+      <c r="L399" s="56"/>
+      <c r="M399" s="56"/>
+      <c r="N399" s="56"/>
+      <c r="O399" s="56"/>
+      <c r="P399" s="56"/>
+      <c r="Q399" s="56"/>
+      <c r="R399" s="56"/>
+      <c r="S399" s="56"/>
+      <c r="T399" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="P369:R369"/>
-    <mergeCell ref="P370:R370"/>
-    <mergeCell ref="L143:M143"/>
-    <mergeCell ref="L144:M144"/>
-    <mergeCell ref="L145:M145"/>
-    <mergeCell ref="L146:M146"/>
-    <mergeCell ref="L147:M147"/>
-    <mergeCell ref="L149:M149"/>
-    <mergeCell ref="L150:M150"/>
-    <mergeCell ref="K368:O368"/>
-    <mergeCell ref="L203:Q203"/>
-    <mergeCell ref="B360:G360"/>
-    <mergeCell ref="B361:G361"/>
-    <mergeCell ref="B362:G362"/>
-    <mergeCell ref="B266:D266"/>
-    <mergeCell ref="G266:H266"/>
-    <mergeCell ref="B280:D280"/>
-    <mergeCell ref="G280:H280"/>
-    <mergeCell ref="B279:D279"/>
-    <mergeCell ref="G279:H279"/>
+    <mergeCell ref="B383:E383"/>
+    <mergeCell ref="F383:H383"/>
+    <mergeCell ref="L383:M383"/>
+    <mergeCell ref="N383:O383"/>
+    <mergeCell ref="F212:G212"/>
+    <mergeCell ref="F213:G213"/>
+    <mergeCell ref="I212:K212"/>
+    <mergeCell ref="I213:K213"/>
+    <mergeCell ref="O212:Q212"/>
+    <mergeCell ref="O213:Q213"/>
+    <mergeCell ref="K369:O369"/>
+    <mergeCell ref="K370:O370"/>
+    <mergeCell ref="P368:R368"/>
+    <mergeCell ref="H360:I360"/>
+    <mergeCell ref="H361:I361"/>
+    <mergeCell ref="H362:I362"/>
+    <mergeCell ref="S383:T383"/>
+    <mergeCell ref="I383:J383"/>
+    <mergeCell ref="P383:Q383"/>
+    <mergeCell ref="I128:O128"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="F138:G138"/>
+    <mergeCell ref="H138:K138"/>
+    <mergeCell ref="L137:M137"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="L138:M138"/>
+    <mergeCell ref="F211:G211"/>
+    <mergeCell ref="I211:K211"/>
+    <mergeCell ref="O211:Q211"/>
+    <mergeCell ref="L148:M148"/>
+    <mergeCell ref="D203:G203"/>
+    <mergeCell ref="H203:K203"/>
+    <mergeCell ref="K124:O124"/>
+    <mergeCell ref="K110:O110"/>
+    <mergeCell ref="K116:O116"/>
+    <mergeCell ref="K113:O113"/>
+    <mergeCell ref="K120:O120"/>
     <mergeCell ref="F143:G143"/>
     <mergeCell ref="F144:G144"/>
     <mergeCell ref="H148:K148"/>
@@ -11447,43 +11503,26 @@
     <mergeCell ref="H145:K145"/>
     <mergeCell ref="H146:K146"/>
     <mergeCell ref="H147:K147"/>
-    <mergeCell ref="K124:O124"/>
-    <mergeCell ref="K110:O110"/>
-    <mergeCell ref="K116:O116"/>
-    <mergeCell ref="K113:O113"/>
-    <mergeCell ref="K120:O120"/>
-    <mergeCell ref="S383:T383"/>
-    <mergeCell ref="I383:J383"/>
-    <mergeCell ref="P383:Q383"/>
-    <mergeCell ref="I128:O128"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="F138:G138"/>
-    <mergeCell ref="H138:K138"/>
-    <mergeCell ref="L137:M137"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="L138:M138"/>
-    <mergeCell ref="F211:G211"/>
-    <mergeCell ref="I211:K211"/>
-    <mergeCell ref="O211:Q211"/>
-    <mergeCell ref="L148:M148"/>
-    <mergeCell ref="D203:G203"/>
-    <mergeCell ref="H203:K203"/>
-    <mergeCell ref="B383:E383"/>
-    <mergeCell ref="F383:H383"/>
-    <mergeCell ref="L383:M383"/>
-    <mergeCell ref="N383:O383"/>
-    <mergeCell ref="F212:G212"/>
-    <mergeCell ref="F213:G213"/>
-    <mergeCell ref="I212:K212"/>
-    <mergeCell ref="I213:K213"/>
-    <mergeCell ref="O212:Q212"/>
-    <mergeCell ref="O213:Q213"/>
-    <mergeCell ref="K369:O369"/>
-    <mergeCell ref="K370:O370"/>
-    <mergeCell ref="P368:R368"/>
-    <mergeCell ref="H360:I360"/>
-    <mergeCell ref="H361:I361"/>
-    <mergeCell ref="H362:I362"/>
+    <mergeCell ref="B360:G360"/>
+    <mergeCell ref="B361:G361"/>
+    <mergeCell ref="B362:G362"/>
+    <mergeCell ref="B266:D266"/>
+    <mergeCell ref="G266:H266"/>
+    <mergeCell ref="B280:D280"/>
+    <mergeCell ref="G280:H280"/>
+    <mergeCell ref="B279:D279"/>
+    <mergeCell ref="G279:H279"/>
+    <mergeCell ref="P369:R369"/>
+    <mergeCell ref="P370:R370"/>
+    <mergeCell ref="L143:M143"/>
+    <mergeCell ref="L144:M144"/>
+    <mergeCell ref="L145:M145"/>
+    <mergeCell ref="L146:M146"/>
+    <mergeCell ref="L147:M147"/>
+    <mergeCell ref="L149:M149"/>
+    <mergeCell ref="L150:M150"/>
+    <mergeCell ref="K368:O368"/>
+    <mergeCell ref="L203:Q203"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
@@ -11492,6 +11531,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:Y18"/>
@@ -11692,446 +11744,160 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист3"/>
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="41"/>
+    <col min="2" max="2" width="9.140625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="114" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="117" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="120" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="79" t="s">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="120" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="80" t="s">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="122" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="123" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="124" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="111" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="91"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="63"/>
     </row>
     <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="92"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="94"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
     </row>
     <row r="9" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="95"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="97"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="69"/>
     </row>
     <row r="10" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="101"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="103"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="106"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="42"/>
+      <c r="B13" s="126"/>
+      <c r="C13" s="127"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="42"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="127"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="86">
+      <c r="A15" s="128">
         <v>42370</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="24" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="140" t="s">
+      <c r="B15" s="129"/>
+      <c r="C15" s="130"/>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="140"/>
-      <c r="C24" s="140"/>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140" t="s">
+      <c r="B16" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="140"/>
-      <c r="G24" s="140"/>
-      <c r="H24" s="140" t="s">
+      <c r="C16" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="140"/>
-      <c r="J24" s="62" t="s">
-        <v>64</v>
+    </row>
+    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="131" t="s">
+        <v>79</v>
       </c>
-      <c r="K24" s="137" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" s="137"/>
-      <c r="M24" s="137" t="s">
-        <v>64</v>
-      </c>
-      <c r="N24" s="137"/>
-      <c r="O24" s="140" t="s">
-        <v>64</v>
-      </c>
-      <c r="P24" s="140"/>
-      <c r="Q24" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="R24" s="137" t="s">
-        <v>64</v>
-      </c>
-      <c r="S24" s="137"/>
-    </row>
-    <row r="25" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="138" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="138"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="138" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
-      <c r="H25" s="138" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" s="138"/>
-      <c r="J25" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="K25" s="139" t="s">
-        <v>64</v>
-      </c>
-      <c r="L25" s="139"/>
-      <c r="M25" s="139" t="s">
-        <v>64</v>
-      </c>
-      <c r="N25" s="139"/>
-      <c r="O25" s="138" t="s">
-        <v>64</v>
-      </c>
-      <c r="P25" s="138"/>
-      <c r="Q25" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="R25" s="139" t="s">
-        <v>64</v>
-      </c>
-      <c r="S25" s="139"/>
-    </row>
-    <row r="26" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="144" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="144"/>
-      <c r="C26" s="144"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="144"/>
-      <c r="G26" s="144"/>
-      <c r="H26" s="144" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26" s="144"/>
-      <c r="J26" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="K26" s="141" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" s="141"/>
-      <c r="M26" s="141" t="s">
-        <v>64</v>
-      </c>
-      <c r="N26" s="141"/>
-      <c r="O26" s="144" t="s">
-        <v>64</v>
-      </c>
-      <c r="P26" s="144"/>
-      <c r="Q26" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="R26" s="141" t="s">
-        <v>64</v>
-      </c>
-      <c r="S26" s="141"/>
-    </row>
-    <row r="27" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="142" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="142"/>
-      <c r="C27" s="142"/>
-      <c r="D27" s="142"/>
-      <c r="E27" s="142" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="142"/>
-      <c r="G27" s="142"/>
-      <c r="H27" s="142" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" s="142"/>
-      <c r="J27" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27" s="143" t="s">
-        <v>64</v>
-      </c>
-      <c r="L27" s="143"/>
-      <c r="M27" s="143" t="s">
-        <v>64</v>
-      </c>
-      <c r="N27" s="143"/>
-      <c r="O27" s="142" t="s">
-        <v>64</v>
-      </c>
-      <c r="P27" s="142"/>
-      <c r="Q27" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="R27" s="143" t="s">
-        <v>64</v>
-      </c>
-      <c r="S27" s="143"/>
-    </row>
-    <row r="28" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="148" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="148"/>
-      <c r="C28" s="148"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="148" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="148"/>
-      <c r="G28" s="148"/>
-      <c r="H28" s="148" t="s">
-        <v>64</v>
-      </c>
-      <c r="I28" s="148"/>
-      <c r="J28" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="K28" s="145" t="s">
-        <v>64</v>
-      </c>
-      <c r="L28" s="145"/>
-      <c r="M28" s="145" t="s">
-        <v>64</v>
-      </c>
-      <c r="N28" s="145"/>
-      <c r="O28" s="148" t="s">
-        <v>64</v>
-      </c>
-      <c r="P28" s="148"/>
-      <c r="Q28" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="R28" s="145" t="s">
-        <v>64</v>
-      </c>
-      <c r="S28" s="145"/>
-    </row>
-    <row r="29" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="146" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="146"/>
-      <c r="C29" s="146"/>
-      <c r="D29" s="146"/>
-      <c r="E29" s="146" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="146"/>
-      <c r="G29" s="146"/>
-      <c r="H29" s="146" t="s">
-        <v>64</v>
-      </c>
-      <c r="I29" s="146"/>
-      <c r="J29" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" s="147" t="s">
-        <v>64</v>
-      </c>
-      <c r="L29" s="147"/>
-      <c r="M29" s="147" t="s">
-        <v>64</v>
-      </c>
-      <c r="N29" s="147"/>
-      <c r="O29" s="146" t="s">
-        <v>64</v>
-      </c>
-      <c r="P29" s="146"/>
-      <c r="Q29" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="R29" s="147" t="s">
-        <v>64</v>
-      </c>
-      <c r="S29" s="147"/>
-    </row>
-    <row r="30" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="150"/>
-      <c r="B30" s="150"/>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
-      <c r="H30" s="150"/>
-      <c r="I30" s="150"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="149"/>
-      <c r="L30" s="149"/>
-      <c r="M30" s="149"/>
-      <c r="N30" s="149"/>
-      <c r="O30" s="150"/>
-      <c r="P30" s="150"/>
-      <c r="Q30" s="59"/>
-      <c r="R30" s="149"/>
-      <c r="S30" s="149"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="133"/>
+    </row>
+    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>